<commit_message>
added file upload functionality
</commit_message>
<xml_diff>
--- a/data/clean 2023 BSC Stats.xlsx
+++ b/data/clean 2023 BSC Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/work/vscode/node1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF96EE5-2D34-BA4E-BA0E-33C28D18EB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DD2F81-8E8C-E24D-BD3F-5F1287D4CAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23 BSC Regular Season Stats" sheetId="1" r:id="rId1"/>
@@ -1922,30 +1922,32 @@
   </sheetPr>
   <dimension ref="A1:AK883"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="Y35" sqref="Y35:AK35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" customWidth="1"/>
-    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" customWidth="1"/>
-    <col min="11" max="11" width="7" customWidth="1"/>
-    <col min="12" max="12" width="8.1640625" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" customWidth="1"/>
-    <col min="15" max="15" width="9.83203125" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" customWidth="1"/>
-    <col min="19" max="19" width="9.33203125" customWidth="1"/>
-    <col min="20" max="20" width="8.1640625" customWidth="1"/>
-    <col min="21" max="21" width="7.33203125" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.6640625" customWidth="1"/>
     <col min="24" max="24" width="19.5" customWidth="1"/>
     <col min="25" max="25" width="11.6640625" customWidth="1"/>
@@ -2069,43 +2071,43 @@
         <v>18</v>
       </c>
       <c r="E4" s="9">
-        <f t="shared" ref="E4:L4" si="0">AVERAGE(E56:E60)</f>
+        <f t="shared" ref="E4" si="0">AVERAGE(E56:E60)</f>
         <v>12.6</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(F56:F60)</f>
         <v>11</v>
       </c>
       <c r="G4" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(G56:G60)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="H4" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(H56:H60)</f>
         <v>8.8000000000000007</v>
       </c>
       <c r="I4" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(I56:I60)</f>
         <v>4</v>
       </c>
       <c r="J4" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(J56:J60)</f>
         <v>1.2</v>
       </c>
       <c r="K4" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(K56:K60)</f>
         <v>0.2</v>
       </c>
       <c r="L4" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(L56:L60)</f>
         <v>2.4</v>
       </c>
       <c r="M4" s="9">
-        <f t="shared" ref="M4:N4" si="1">AVERAGE(M56:M60)+P4</f>
+        <f>AVERAGE(M56:M60)+P4</f>
         <v>14</v>
       </c>
       <c r="N4" s="9">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(N56:N60)+Q4</f>
         <v>5.4</v>
       </c>
       <c r="O4" s="10" t="e">
@@ -2113,11 +2115,11 @@
         <v>#REF!</v>
       </c>
       <c r="P4" s="9">
-        <f t="shared" ref="P4:Q4" si="2">AVERAGE(P56:P60)</f>
+        <f t="shared" ref="P4:Q4" si="1">AVERAGE(P56:P60)</f>
         <v>1.4</v>
       </c>
       <c r="Q4" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="R4" s="10" t="e">
@@ -2125,15 +2127,15 @@
         <v>#REF!</v>
       </c>
       <c r="S4" s="9">
-        <f t="shared" ref="S4:T4" si="3">AVERAGE(S56:S60)</f>
+        <f t="shared" ref="S4:T4" si="2">AVERAGE(S56:S60)</f>
         <v>3.2</v>
       </c>
       <c r="T4" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.4</v>
       </c>
       <c r="U4" s="10">
-        <f t="shared" ref="U4:U35" si="4">T4/S4</f>
+        <f t="shared" ref="U4:U35" si="3">T4/S4</f>
         <v>0.43749999999999994</v>
       </c>
       <c r="V4" s="10">
@@ -2150,35 +2152,35 @@
         <v>19</v>
       </c>
       <c r="E5" s="11">
-        <f t="shared" ref="E5:L5" si="5">AVERAGE(E61:E65)</f>
+        <f t="shared" ref="E5" si="4">AVERAGE(E61:E65)</f>
         <v>16.2</v>
       </c>
       <c r="F5" s="11">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(F61:F65)</f>
         <v>13</v>
       </c>
       <c r="G5" s="11">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(G61:G65)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="H5" s="11">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(H61:H65)</f>
         <v>8.6</v>
       </c>
       <c r="I5" s="11">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(I61:I65)</f>
         <v>3.8</v>
       </c>
       <c r="J5" s="11">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(J61:J65)</f>
         <v>0.4</v>
       </c>
       <c r="K5" s="11">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(K61:K65)</f>
         <v>1.6</v>
       </c>
       <c r="L5" s="11">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(L61:L65)</f>
         <v>2.8</v>
       </c>
       <c r="M5" s="11">
@@ -2194,11 +2196,11 @@
         <v>#REF!</v>
       </c>
       <c r="P5" s="11">
-        <f t="shared" ref="P5:Q5" si="6">AVERAGE(P61:P65)</f>
+        <f t="shared" ref="P5:Q5" si="5">AVERAGE(P61:P65)</f>
         <v>9.4</v>
       </c>
       <c r="Q5" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.4</v>
       </c>
       <c r="R5" s="1" t="e">
@@ -2206,19 +2208,19 @@
         <v>#REF!</v>
       </c>
       <c r="S5" s="11">
-        <f t="shared" ref="S5:T5" si="7">AVERAGE(S61:S65)</f>
+        <f t="shared" ref="S5:T5" si="6">AVERAGE(S61:S65)</f>
         <v>3.4</v>
       </c>
       <c r="T5" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.6</v>
       </c>
       <c r="U5" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="V5" s="1">
-        <f t="shared" ref="V5:V35" si="8">E5/(2*(M5+0.44*S5))</f>
+        <f>E5/(2*(M5+0.44*S5))</f>
         <v>0.36993058092802339</v>
       </c>
       <c r="Z5" s="11"/>
@@ -2231,35 +2233,35 @@
         <v>20</v>
       </c>
       <c r="E6" s="11">
-        <f t="shared" ref="E6:L6" si="9">AVERAGE(E66:E70)</f>
+        <f t="shared" ref="E6" si="7">AVERAGE(E66:E70)</f>
         <v>8.4</v>
       </c>
       <c r="F6" s="11">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(F66:F70)</f>
         <v>6.2</v>
       </c>
       <c r="G6" s="11">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(G66:G70)</f>
         <v>0.4</v>
       </c>
       <c r="H6" s="11">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(H66:H70)</f>
         <v>5.8</v>
       </c>
       <c r="I6" s="11">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(I66:I70)</f>
         <v>1.8</v>
       </c>
       <c r="J6" s="11">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(J66:J70)</f>
         <v>1.4</v>
       </c>
       <c r="K6" s="11">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(K66:K70)</f>
         <v>0.4</v>
       </c>
       <c r="L6" s="11">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(L66:L70)</f>
         <v>1.4</v>
       </c>
       <c r="M6" s="11">
@@ -2275,11 +2277,11 @@
         <v>#REF!</v>
       </c>
       <c r="P6" s="11">
-        <f t="shared" ref="P6:Q6" si="10">AVERAGE(P66:P70)</f>
+        <f t="shared" ref="P6:Q6" si="8">AVERAGE(P66:P70)</f>
         <v>7.2</v>
       </c>
       <c r="Q6" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1.8</v>
       </c>
       <c r="R6" s="1" t="e">
@@ -2287,19 +2289,19 @@
         <v>#REF!</v>
       </c>
       <c r="S6" s="11">
-        <f t="shared" ref="S6:T6" si="11">AVERAGE(S66:S70)</f>
+        <f t="shared" ref="S6:T6" si="9">AVERAGE(S66:S70)</f>
         <v>0.6</v>
       </c>
       <c r="T6" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0.2</v>
       </c>
       <c r="U6" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333337</v>
       </c>
       <c r="V6" s="1">
-        <f t="shared" si="8"/>
+        <f>E6/(2*(M6+0.44*S6))</f>
         <v>0.29863481228668942</v>
       </c>
       <c r="AA6" s="6"/>
@@ -2311,35 +2313,35 @@
         <v>21</v>
       </c>
       <c r="E7" s="14">
-        <f t="shared" ref="E7:L7" si="12">AVERAGE(E71:E75)</f>
+        <f t="shared" ref="E7" si="10">AVERAGE(E71:E75)</f>
         <v>7</v>
       </c>
       <c r="F7" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(F71:F75)</f>
         <v>7</v>
       </c>
       <c r="G7" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(G71:G75)</f>
         <v>1</v>
       </c>
       <c r="H7" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(H71:H75)</f>
         <v>6</v>
       </c>
       <c r="I7" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(I71:I75)</f>
         <v>0.6</v>
       </c>
       <c r="J7" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(J71:J75)</f>
         <v>0.4</v>
       </c>
       <c r="K7" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(K71:K75)</f>
         <v>0</v>
       </c>
       <c r="L7" s="14">
-        <f t="shared" si="12"/>
+        <f>AVERAGE(L71:L75)</f>
         <v>1.4</v>
       </c>
       <c r="M7" s="14">
@@ -2355,11 +2357,11 @@
         <v>#REF!</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:Q7" si="13">AVERAGE(P71:P75)</f>
+        <f t="shared" ref="P7:Q7" si="11">AVERAGE(P71:P75)</f>
         <v>0.6</v>
       </c>
       <c r="Q7" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0.2</v>
       </c>
       <c r="R7" s="15" t="e">
@@ -2367,19 +2369,19 @@
         <v>#REF!</v>
       </c>
       <c r="S7" s="14">
-        <f t="shared" ref="S7:T7" si="14">AVERAGE(S71:S75)</f>
+        <f t="shared" ref="S7:T7" si="12">AVERAGE(S71:S75)</f>
         <v>1.8</v>
       </c>
       <c r="T7" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1.2</v>
       </c>
       <c r="U7" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="V7" s="15">
-        <f t="shared" si="8"/>
+        <f>E7/(2*(M7+0.44*S7))</f>
         <v>0.44917864476386038</v>
       </c>
       <c r="AA7" s="6"/>
@@ -2391,35 +2393,35 @@
         <v>22</v>
       </c>
       <c r="E8" s="11">
-        <f t="shared" ref="E8:L8" si="15">AVERAGE(E76:E80)</f>
+        <f t="shared" ref="E8" si="13">AVERAGE(E76:E80)</f>
         <v>14.8</v>
       </c>
       <c r="F8" s="11">
-        <f t="shared" si="15"/>
+        <f>AVERAGE(F76:F80)</f>
         <v>7.8</v>
       </c>
       <c r="G8" s="11">
-        <f t="shared" si="15"/>
+        <f>AVERAGE(G76:G80)</f>
         <v>0.2</v>
       </c>
       <c r="H8" s="11">
-        <f t="shared" si="15"/>
+        <f>AVERAGE(H76:H80)</f>
         <v>7.6</v>
       </c>
       <c r="I8" s="11">
-        <f t="shared" si="15"/>
+        <f>AVERAGE(I76:I80)</f>
         <v>3.4</v>
       </c>
       <c r="J8" s="11">
-        <f t="shared" si="15"/>
+        <f>AVERAGE(J76:J80)</f>
         <v>0.6</v>
       </c>
       <c r="K8" s="11">
-        <f t="shared" si="15"/>
+        <f>AVERAGE(K76:K80)</f>
         <v>0.6</v>
       </c>
       <c r="L8" s="11">
-        <f t="shared" si="15"/>
+        <f>AVERAGE(L76:L80)</f>
         <v>2.6</v>
       </c>
       <c r="M8" s="11">
@@ -2435,11 +2437,11 @@
         <v>#REF!</v>
       </c>
       <c r="P8" s="11">
-        <f t="shared" ref="P8:Q8" si="16">AVERAGE(P76:P80)</f>
+        <f t="shared" ref="P8:Q8" si="14">AVERAGE(P76:P80)</f>
         <v>8.4</v>
       </c>
       <c r="Q8" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>1.4</v>
       </c>
       <c r="R8" s="1" t="e">
@@ -2447,19 +2449,19 @@
         <v>#REF!</v>
       </c>
       <c r="S8" s="11">
-        <f t="shared" ref="S8:T8" si="17">AVERAGE(S76:S80)</f>
+        <f t="shared" ref="S8:T8" si="15">AVERAGE(S76:S80)</f>
         <v>2</v>
       </c>
       <c r="T8" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="U8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="V8" s="1">
-        <f t="shared" si="8"/>
+        <f>E8/(2*(M8+0.44*S8))</f>
         <v>0.39194915254237295</v>
       </c>
       <c r="AA8" s="6"/>
@@ -2471,35 +2473,35 @@
         <v>23</v>
       </c>
       <c r="E9" s="11">
-        <f t="shared" ref="E9:L9" si="18">AVERAGE(E81:E85)</f>
+        <f t="shared" ref="E9" si="16">AVERAGE(E81:E85)</f>
         <v>26.2</v>
       </c>
       <c r="F9" s="11">
-        <f t="shared" si="18"/>
+        <f>AVERAGE(F81:F85)</f>
         <v>6.6</v>
       </c>
       <c r="G9" s="11">
-        <f t="shared" si="18"/>
+        <f>AVERAGE(G81:G85)</f>
         <v>2</v>
       </c>
       <c r="H9" s="11">
-        <f t="shared" si="18"/>
+        <f>AVERAGE(H81:H85)</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="I9" s="11">
-        <f t="shared" si="18"/>
+        <f>AVERAGE(I81:I85)</f>
         <v>1.6</v>
       </c>
       <c r="J9" s="11">
-        <f t="shared" si="18"/>
+        <f>AVERAGE(J81:J85)</f>
         <v>1.2</v>
       </c>
       <c r="K9" s="11">
-        <f t="shared" si="18"/>
+        <f>AVERAGE(K81:K85)</f>
         <v>0.8</v>
       </c>
       <c r="L9" s="11">
-        <f t="shared" si="18"/>
+        <f>AVERAGE(L81:L85)</f>
         <v>1.6</v>
       </c>
       <c r="M9" s="11">
@@ -2515,11 +2517,11 @@
         <v>#REF!</v>
       </c>
       <c r="P9" s="11">
-        <f t="shared" ref="P9:Q9" si="19">AVERAGE(P81:P85)</f>
+        <f t="shared" ref="P9:Q9" si="17">AVERAGE(P81:P85)</f>
         <v>12</v>
       </c>
       <c r="Q9" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>4.2</v>
       </c>
       <c r="R9" s="1" t="e">
@@ -2527,19 +2529,19 @@
         <v>#REF!</v>
       </c>
       <c r="S9" s="11">
-        <f t="shared" ref="S9:T9" si="20">AVERAGE(S81:S85)</f>
+        <f t="shared" ref="S9:T9" si="18">AVERAGE(S81:S85)</f>
         <v>5.6</v>
       </c>
       <c r="T9" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>3.6</v>
       </c>
       <c r="U9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.6428571428571429</v>
       </c>
       <c r="V9" s="1">
-        <f t="shared" si="8"/>
+        <f>E9/(2*(M9+0.44*S9))</f>
         <v>0.49129912991299135</v>
       </c>
       <c r="AA9" s="6"/>
@@ -2551,35 +2553,35 @@
         <v>24</v>
       </c>
       <c r="E10" s="11">
-        <f t="shared" ref="E10:L10" si="21">AVERAGE(E86:E90)</f>
+        <f t="shared" ref="E10" si="19">AVERAGE(E86:E90)</f>
         <v>5.6</v>
       </c>
       <c r="F10" s="11">
-        <f t="shared" si="21"/>
+        <f>AVERAGE(F86:F90)</f>
         <v>9.6</v>
       </c>
       <c r="G10" s="11">
-        <f t="shared" si="21"/>
+        <f>AVERAGE(G86:G90)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="H10" s="11">
-        <f t="shared" si="21"/>
+        <f>AVERAGE(H86:H90)</f>
         <v>5.2</v>
       </c>
       <c r="I10" s="11">
-        <f t="shared" si="21"/>
+        <f>AVERAGE(I86:I90)</f>
         <v>1.6</v>
       </c>
       <c r="J10" s="11">
-        <f t="shared" si="21"/>
+        <f>AVERAGE(J86:J90)</f>
         <v>0.4</v>
       </c>
       <c r="K10" s="11">
-        <f t="shared" si="21"/>
+        <f>AVERAGE(K86:K90)</f>
         <v>0.2</v>
       </c>
       <c r="L10" s="11">
-        <f t="shared" si="21"/>
+        <f>AVERAGE(L86:L90)</f>
         <v>0.8</v>
       </c>
       <c r="M10" s="11">
@@ -2595,11 +2597,11 @@
         <v>#REF!</v>
       </c>
       <c r="P10" s="11">
-        <f t="shared" ref="P10:Q10" si="22">AVERAGE(P86:P90)</f>
+        <f t="shared" ref="P10:Q10" si="20">AVERAGE(P86:P90)</f>
         <v>1.4</v>
       </c>
       <c r="Q10" s="11">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R10" s="1" t="e">
@@ -2607,19 +2609,19 @@
         <v>#REF!</v>
       </c>
       <c r="S10" s="11">
-        <f t="shared" ref="S10:T10" si="23">AVERAGE(S86:S90)</f>
+        <f t="shared" ref="S10:T10" si="21">AVERAGE(S86:S90)</f>
         <v>1.6</v>
       </c>
       <c r="T10" s="11">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.8</v>
       </c>
       <c r="U10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="V10" s="1">
-        <f t="shared" si="8"/>
+        <f>E10/(2*(M10+0.44*S10))</f>
         <v>0.30755711775043931</v>
       </c>
       <c r="AA10" s="6"/>
@@ -2631,35 +2633,35 @@
         <v>25</v>
       </c>
       <c r="E11" s="14">
-        <f t="shared" ref="E11:L11" si="24">AVERAGE(E91:E95)</f>
+        <f t="shared" ref="E11" si="22">AVERAGE(E91:E95)</f>
         <v>3.8</v>
       </c>
       <c r="F11" s="14">
-        <f t="shared" si="24"/>
+        <f>AVERAGE(F91:F95)</f>
         <v>5.6</v>
       </c>
       <c r="G11" s="14">
-        <f t="shared" si="24"/>
+        <f>AVERAGE(G91:G95)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="H11" s="14">
-        <f t="shared" si="24"/>
+        <f>AVERAGE(H91:H95)</f>
         <v>3.4</v>
       </c>
       <c r="I11" s="14">
-        <f t="shared" si="24"/>
+        <f>AVERAGE(I91:I95)</f>
         <v>1.8</v>
       </c>
       <c r="J11" s="14">
-        <f t="shared" si="24"/>
+        <f>AVERAGE(J91:J95)</f>
         <v>0.8</v>
       </c>
       <c r="K11" s="14">
-        <f t="shared" si="24"/>
+        <f>AVERAGE(K91:K95)</f>
         <v>0.8</v>
       </c>
       <c r="L11" s="14">
-        <f t="shared" si="24"/>
+        <f>AVERAGE(L91:L95)</f>
         <v>0.4</v>
       </c>
       <c r="M11" s="14">
@@ -2675,11 +2677,11 @@
         <v>#REF!</v>
       </c>
       <c r="P11" s="14">
-        <f t="shared" ref="P11:Q11" si="25">AVERAGE(P91:P95)</f>
+        <f t="shared" ref="P11:Q11" si="23">AVERAGE(P91:P95)</f>
         <v>1.2</v>
       </c>
       <c r="Q11" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="R11" s="15" t="e">
@@ -2687,19 +2689,19 @@
         <v>#REF!</v>
       </c>
       <c r="S11" s="14">
-        <f t="shared" ref="S11:T11" si="26">AVERAGE(S91:S95)</f>
+        <f t="shared" ref="S11:T11" si="24">AVERAGE(S91:S95)</f>
         <v>2.4</v>
       </c>
       <c r="T11" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>0.8</v>
       </c>
       <c r="U11" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333337</v>
       </c>
       <c r="V11" s="15">
-        <f t="shared" si="8"/>
+        <f>E11/(2*(M11+0.44*S11))</f>
         <v>0.26927437641723356</v>
       </c>
       <c r="Z11" s="11"/>
@@ -2712,35 +2714,35 @@
         <v>26</v>
       </c>
       <c r="E12" s="11">
-        <f t="shared" ref="E12:L12" si="27">AVERAGE(E96:E100)</f>
+        <f t="shared" ref="E12" si="25">AVERAGE(E96:E100)</f>
         <v>25.6</v>
       </c>
       <c r="F12" s="11">
-        <f t="shared" si="27"/>
+        <f>AVERAGE(F96:F100)</f>
         <v>11.4</v>
       </c>
       <c r="G12" s="11">
-        <f t="shared" si="27"/>
+        <f>AVERAGE(G96:G100)</f>
         <v>1.8</v>
       </c>
       <c r="H12" s="11">
-        <f t="shared" si="27"/>
+        <f>AVERAGE(H96:H100)</f>
         <v>9.6</v>
       </c>
       <c r="I12" s="11">
-        <f t="shared" si="27"/>
+        <f>AVERAGE(I96:I100)</f>
         <v>1.2</v>
       </c>
       <c r="J12" s="11">
-        <f t="shared" si="27"/>
+        <f>AVERAGE(J96:J100)</f>
         <v>0.4</v>
       </c>
       <c r="K12" s="11">
-        <f t="shared" si="27"/>
+        <f>AVERAGE(K96:K100)</f>
         <v>0.6</v>
       </c>
       <c r="L12" s="11">
-        <f t="shared" si="27"/>
+        <f>AVERAGE(L96:L100)</f>
         <v>1.8</v>
       </c>
       <c r="M12" s="11">
@@ -2756,11 +2758,11 @@
         <v>#REF!</v>
       </c>
       <c r="P12" s="11">
-        <f t="shared" ref="P12:Q12" si="28">AVERAGE(P96:P100)</f>
+        <f t="shared" ref="P12:Q12" si="26">AVERAGE(P96:P100)</f>
         <v>16</v>
       </c>
       <c r="Q12" s="11">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>3.4</v>
       </c>
       <c r="R12" s="1" t="e">
@@ -2768,19 +2770,19 @@
         <v>#REF!</v>
       </c>
       <c r="S12" s="11">
-        <f t="shared" ref="S12:T12" si="29">AVERAGE(S96:S100)</f>
+        <f t="shared" ref="S12:T12" si="27">AVERAGE(S96:S100)</f>
         <v>5.4</v>
       </c>
       <c r="T12" s="11">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>3.8</v>
       </c>
       <c r="U12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.70370370370370361</v>
       </c>
       <c r="V12" s="1">
-        <f t="shared" si="8"/>
+        <f>E12/(2*(M12+0.44*S12))</f>
         <v>0.40537116797567774</v>
       </c>
       <c r="Z12" s="11"/>
@@ -2793,35 +2795,35 @@
         <v>27</v>
       </c>
       <c r="E13" s="11">
-        <f t="shared" ref="E13:L13" si="30">AVERAGE(E101:E105)</f>
+        <f t="shared" ref="E13" si="28">AVERAGE(E101:E105)</f>
         <v>17.600000000000001</v>
       </c>
       <c r="F13" s="11">
-        <f t="shared" si="30"/>
+        <f>AVERAGE(F101:F105)</f>
         <v>11.8</v>
       </c>
       <c r="G13" s="11">
-        <f t="shared" si="30"/>
+        <f>AVERAGE(G101:G105)</f>
         <v>2.8</v>
       </c>
       <c r="H13" s="11">
-        <f t="shared" si="30"/>
+        <f>AVERAGE(H101:H105)</f>
         <v>9</v>
       </c>
       <c r="I13" s="11">
-        <f t="shared" si="30"/>
+        <f>AVERAGE(I101:I105)</f>
         <v>2.6</v>
       </c>
       <c r="J13" s="11">
-        <f t="shared" si="30"/>
+        <f>AVERAGE(J101:J105)</f>
         <v>2</v>
       </c>
       <c r="K13" s="11">
-        <f t="shared" si="30"/>
+        <f>AVERAGE(K101:K105)</f>
         <v>0.2</v>
       </c>
       <c r="L13" s="11">
-        <f t="shared" si="30"/>
+        <f>AVERAGE(L101:L105)</f>
         <v>2.4</v>
       </c>
       <c r="M13" s="11">
@@ -2837,11 +2839,11 @@
         <v>#REF!</v>
       </c>
       <c r="P13" s="11">
-        <f t="shared" ref="P13:Q13" si="31">AVERAGE(P101:P105)</f>
+        <f t="shared" ref="P13:Q13" si="29">AVERAGE(P101:P105)</f>
         <v>6.4</v>
       </c>
       <c r="Q13" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>1.8</v>
       </c>
       <c r="R13" s="1" t="e">
@@ -2849,19 +2851,19 @@
         <v>#REF!</v>
       </c>
       <c r="S13" s="11">
-        <f t="shared" ref="S13:T13" si="32">AVERAGE(S101:S105)</f>
+        <f t="shared" ref="S13:T13" si="30">AVERAGE(S101:S105)</f>
         <v>1.8</v>
       </c>
       <c r="T13" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>1.4</v>
       </c>
       <c r="U13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.77777777777777768</v>
       </c>
       <c r="V13" s="1">
-        <f t="shared" si="8"/>
+        <f>E13/(2*(M13+0.44*S13))</f>
         <v>0.45379537953795374</v>
       </c>
       <c r="Z13" s="11"/>
@@ -2873,35 +2875,35 @@
         <v>28</v>
       </c>
       <c r="E14" s="11">
-        <f t="shared" ref="E14:L14" si="33">AVERAGE(E106:E110)</f>
+        <f t="shared" ref="E14" si="31">AVERAGE(E106:E110)</f>
         <v>3.2</v>
       </c>
       <c r="F14" s="11">
-        <f t="shared" si="33"/>
+        <f>AVERAGE(F106:F110)</f>
         <v>4</v>
       </c>
       <c r="G14" s="11">
-        <f t="shared" si="33"/>
+        <f>AVERAGE(G106:G110)</f>
         <v>1.4</v>
       </c>
       <c r="H14" s="11">
-        <f t="shared" si="33"/>
+        <f>AVERAGE(H106:H110)</f>
         <v>2.6</v>
       </c>
       <c r="I14" s="11">
-        <f t="shared" si="33"/>
+        <f>AVERAGE(I106:I110)</f>
         <v>3</v>
       </c>
       <c r="J14" s="11">
-        <f t="shared" si="33"/>
+        <f>AVERAGE(J106:J110)</f>
         <v>1</v>
       </c>
       <c r="K14" s="11">
-        <f t="shared" si="33"/>
+        <f>AVERAGE(K106:K110)</f>
         <v>1</v>
       </c>
       <c r="L14" s="11">
-        <f t="shared" si="33"/>
+        <f>AVERAGE(L106:L110)</f>
         <v>1.2</v>
       </c>
       <c r="M14" s="11">
@@ -2917,11 +2919,11 @@
         <v>#REF!</v>
       </c>
       <c r="P14" s="11">
-        <f t="shared" ref="P14:Q14" si="34">AVERAGE(P106:P110)</f>
+        <f t="shared" ref="P14:Q14" si="32">AVERAGE(P106:P110)</f>
         <v>6</v>
       </c>
       <c r="Q14" s="11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0.8</v>
       </c>
       <c r="R14" s="1" t="e">
@@ -2929,19 +2931,19 @@
         <v>#REF!</v>
       </c>
       <c r="S14" s="11">
-        <f t="shared" ref="S14:T14" si="35">AVERAGE(S106:S110)</f>
+        <f t="shared" ref="S14:T14" si="33">AVERAGE(S106:S110)</f>
         <v>0</v>
       </c>
       <c r="T14" s="11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="U14" s="1" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V14" s="1">
-        <f t="shared" si="8"/>
+        <f>E14/(2*(M14+0.44*S14))</f>
         <v>0.19512195121951223</v>
       </c>
       <c r="Z14" s="11"/>
@@ -2953,35 +2955,35 @@
         <v>29</v>
       </c>
       <c r="E15" s="14">
-        <f t="shared" ref="E15:L15" si="36">AVERAGE(E111:E115)</f>
+        <f t="shared" ref="E15" si="34">AVERAGE(E111:E115)</f>
         <v>3.2</v>
       </c>
       <c r="F15" s="14">
-        <f t="shared" si="36"/>
+        <f>AVERAGE(F111:F115)</f>
         <v>6</v>
       </c>
       <c r="G15" s="14">
-        <f t="shared" si="36"/>
+        <f>AVERAGE(G111:G115)</f>
         <v>2</v>
       </c>
       <c r="H15" s="14">
-        <f t="shared" si="36"/>
+        <f>AVERAGE(H111:H115)</f>
         <v>4</v>
       </c>
       <c r="I15" s="14">
-        <f t="shared" si="36"/>
+        <f>AVERAGE(I111:I115)</f>
         <v>1.4</v>
       </c>
       <c r="J15" s="14">
-        <f t="shared" si="36"/>
+        <f>AVERAGE(J111:J115)</f>
         <v>0.4</v>
       </c>
       <c r="K15" s="14">
-        <f t="shared" si="36"/>
+        <f>AVERAGE(K111:K115)</f>
         <v>0.4</v>
       </c>
       <c r="L15" s="14">
-        <f t="shared" si="36"/>
+        <f>AVERAGE(L111:L115)</f>
         <v>0.6</v>
       </c>
       <c r="M15" s="14">
@@ -2997,11 +2999,11 @@
         <v>#REF!</v>
       </c>
       <c r="P15" s="14">
-        <f t="shared" ref="P15:Q15" si="37">AVERAGE(P111:P115)</f>
+        <f t="shared" ref="P15:Q15" si="35">AVERAGE(P111:P115)</f>
         <v>1.8</v>
       </c>
       <c r="Q15" s="14">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="R15" s="15" t="e">
@@ -3009,19 +3011,19 @@
         <v>#REF!</v>
       </c>
       <c r="S15" s="14">
-        <f t="shared" ref="S15:T15" si="38">AVERAGE(S111:S115)</f>
+        <f t="shared" ref="S15:T15" si="36">AVERAGE(S111:S115)</f>
         <v>1.6</v>
       </c>
       <c r="T15" s="14">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>0.2</v>
       </c>
       <c r="U15" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
       <c r="V15" s="15">
-        <f t="shared" si="8"/>
+        <f>E15/(2*(M15+0.44*S15))</f>
         <v>0.29069767441860467</v>
       </c>
       <c r="W15" s="11"/>
@@ -3034,35 +3036,35 @@
         <v>30</v>
       </c>
       <c r="E16" s="11">
-        <f t="shared" ref="E16:L16" si="39">AVERAGE(E116:E120)</f>
+        <f t="shared" ref="E16" si="37">AVERAGE(E116:E120)</f>
         <v>20</v>
       </c>
       <c r="F16" s="11">
-        <f t="shared" si="39"/>
+        <f>AVERAGE(F116:F120)</f>
         <v>12.2</v>
       </c>
       <c r="G16" s="11">
-        <f t="shared" si="39"/>
+        <f>AVERAGE(G116:G120)</f>
         <v>2.8</v>
       </c>
       <c r="H16" s="11">
-        <f t="shared" si="39"/>
+        <f>AVERAGE(H116:H120)</f>
         <v>9.4</v>
       </c>
       <c r="I16" s="11">
-        <f t="shared" si="39"/>
+        <f>AVERAGE(I116:I120)</f>
         <v>2.8</v>
       </c>
       <c r="J16" s="11">
-        <f t="shared" si="39"/>
+        <f>AVERAGE(J116:J120)</f>
         <v>1.2</v>
       </c>
       <c r="K16" s="11">
-        <f t="shared" si="39"/>
+        <f>AVERAGE(K116:K120)</f>
         <v>0.6</v>
       </c>
       <c r="L16" s="11">
-        <f t="shared" si="39"/>
+        <f>AVERAGE(L116:L120)</f>
         <v>3</v>
       </c>
       <c r="M16" s="11">
@@ -3078,11 +3080,11 @@
         <v>#REF!</v>
       </c>
       <c r="P16" s="11">
-        <f t="shared" ref="P16:Q16" si="40">AVERAGE(P116:P120)</f>
+        <f t="shared" ref="P16:Q16" si="38">AVERAGE(P116:P120)</f>
         <v>7</v>
       </c>
       <c r="Q16" s="11">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>1.6</v>
       </c>
       <c r="R16" s="1" t="e">
@@ -3090,19 +3092,19 @@
         <v>#REF!</v>
       </c>
       <c r="S16" s="11">
-        <f t="shared" ref="S16:T16" si="41">AVERAGE(S116:S120)</f>
+        <f t="shared" ref="S16:T16" si="39">AVERAGE(S116:S120)</f>
         <v>3.8</v>
       </c>
       <c r="T16" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>2.4</v>
       </c>
       <c r="U16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.63157894736842102</v>
       </c>
       <c r="V16" s="1">
-        <f t="shared" si="8"/>
+        <f>E16/(2*(M16+0.44*S16))</f>
         <v>0.42603953646898429</v>
       </c>
       <c r="X16" s="11"/>
@@ -3115,35 +3117,35 @@
         <v>31</v>
       </c>
       <c r="E17" s="11">
-        <f t="shared" ref="E17:L17" si="42">AVERAGE(E121:E125)</f>
+        <f t="shared" ref="E17" si="40">AVERAGE(E121:E125)</f>
         <v>19.399999999999999</v>
       </c>
       <c r="F17" s="11">
-        <f t="shared" si="42"/>
+        <f>AVERAGE(F121:F125)</f>
         <v>11</v>
       </c>
       <c r="G17" s="11">
-        <f t="shared" si="42"/>
+        <f>AVERAGE(G121:G125)</f>
         <v>2</v>
       </c>
       <c r="H17" s="11">
-        <f t="shared" si="42"/>
+        <f>AVERAGE(H121:H125)</f>
         <v>9</v>
       </c>
       <c r="I17" s="11">
-        <f t="shared" si="42"/>
+        <f>AVERAGE(I121:I125)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="J17" s="11">
-        <f t="shared" si="42"/>
+        <f>AVERAGE(J121:J125)</f>
         <v>3</v>
       </c>
       <c r="K17" s="11">
-        <f t="shared" si="42"/>
+        <f>AVERAGE(K121:K125)</f>
         <v>2.4</v>
       </c>
       <c r="L17" s="11">
-        <f t="shared" si="42"/>
+        <f>AVERAGE(L121:L125)</f>
         <v>3.6</v>
       </c>
       <c r="M17" s="11">
@@ -3159,11 +3161,11 @@
         <v>#REF!</v>
       </c>
       <c r="P17" s="11">
-        <f t="shared" ref="P17:Q17" si="43">AVERAGE(P121:P125)</f>
+        <f t="shared" ref="P17:Q17" si="41">AVERAGE(P121:P125)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="Q17" s="11">
-        <f t="shared" si="43"/>
+        <f t="shared" si="41"/>
         <v>1.2</v>
       </c>
       <c r="R17" s="1" t="e">
@@ -3171,19 +3173,19 @@
         <v>#REF!</v>
       </c>
       <c r="S17" s="11">
-        <f t="shared" ref="S17:T17" si="44">AVERAGE(S121:S125)</f>
+        <f t="shared" ref="S17:T17" si="42">AVERAGE(S121:S125)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="T17" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="42"/>
         <v>3.4</v>
       </c>
       <c r="U17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.7727272727272726</v>
       </c>
       <c r="V17" s="1">
-        <f t="shared" si="8"/>
+        <f>E17/(2*(M17+0.44*S17))</f>
         <v>0.47234125438254765</v>
       </c>
       <c r="X17" s="11"/>
@@ -3196,35 +3198,35 @@
         <v>32</v>
       </c>
       <c r="E18" s="11">
-        <f t="shared" ref="E18:L18" si="45">AVERAGE(E126:E130)</f>
+        <f t="shared" ref="E18" si="43">AVERAGE(E126:E130)</f>
         <v>4</v>
       </c>
       <c r="F18" s="11">
-        <f t="shared" si="45"/>
+        <f>AVERAGE(F126:F130)</f>
         <v>7.75</v>
       </c>
       <c r="G18" s="11">
-        <f t="shared" si="45"/>
+        <f>AVERAGE(G126:G130)</f>
         <v>1.75</v>
       </c>
       <c r="H18" s="11">
-        <f t="shared" si="45"/>
+        <f>AVERAGE(H126:H130)</f>
         <v>6</v>
       </c>
       <c r="I18" s="11">
-        <f t="shared" si="45"/>
+        <f>AVERAGE(I126:I130)</f>
         <v>3.25</v>
       </c>
       <c r="J18" s="11">
-        <f t="shared" si="45"/>
+        <f>AVERAGE(J126:J130)</f>
         <v>1</v>
       </c>
       <c r="K18" s="11">
-        <f t="shared" si="45"/>
+        <f>AVERAGE(K126:K130)</f>
         <v>0.5</v>
       </c>
       <c r="L18" s="11">
-        <f t="shared" si="45"/>
+        <f>AVERAGE(L126:L130)</f>
         <v>3</v>
       </c>
       <c r="M18" s="11">
@@ -3240,11 +3242,11 @@
         <v>#REF!</v>
       </c>
       <c r="P18" s="11">
-        <f t="shared" ref="P18:Q18" si="46">AVERAGE(P126:P130)</f>
+        <f t="shared" ref="P18:Q18" si="44">AVERAGE(P126:P130)</f>
         <v>2</v>
       </c>
       <c r="Q18" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="R18" s="1" t="e">
@@ -3252,19 +3254,19 @@
         <v>#REF!</v>
       </c>
       <c r="S18" s="11">
-        <f t="shared" ref="S18:T18" si="47">AVERAGE(S126:S130)</f>
+        <f t="shared" ref="S18:T18" si="45">AVERAGE(S126:S130)</f>
         <v>0</v>
       </c>
       <c r="T18" s="11">
-        <f t="shared" si="47"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="U18" s="1" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V18" s="1">
-        <f t="shared" si="8"/>
+        <f>E18/(2*(M18+0.44*S18))</f>
         <v>0.1951219512195122</v>
       </c>
       <c r="X18" s="11"/>
@@ -3277,35 +3279,35 @@
         <v>33</v>
       </c>
       <c r="E19" s="14">
-        <f t="shared" ref="E19:L19" si="48">AVERAGE(E131:E135)</f>
+        <f t="shared" ref="E19" si="46">AVERAGE(E131:E135)</f>
         <v>4.5</v>
       </c>
       <c r="F19" s="14">
-        <f t="shared" si="48"/>
+        <f>AVERAGE(F131:F135)</f>
         <v>5.5</v>
       </c>
       <c r="G19" s="14">
-        <f t="shared" si="48"/>
+        <f>AVERAGE(G131:G135)</f>
         <v>1.75</v>
       </c>
       <c r="H19" s="14">
-        <f t="shared" si="48"/>
+        <f>AVERAGE(H131:H135)</f>
         <v>3.75</v>
       </c>
       <c r="I19" s="14">
-        <f t="shared" si="48"/>
+        <f>AVERAGE(I131:I135)</f>
         <v>0.75</v>
       </c>
       <c r="J19" s="14">
-        <f t="shared" si="48"/>
+        <f>AVERAGE(J131:J135)</f>
         <v>0.75</v>
       </c>
       <c r="K19" s="14">
-        <f t="shared" si="48"/>
+        <f>AVERAGE(K131:K135)</f>
         <v>0.75</v>
       </c>
       <c r="L19" s="14">
-        <f t="shared" si="48"/>
+        <f>AVERAGE(L131:L135)</f>
         <v>0.75</v>
       </c>
       <c r="M19" s="14">
@@ -3321,11 +3323,11 @@
         <v>#REF!</v>
       </c>
       <c r="P19" s="14">
-        <f t="shared" ref="P19:Q19" si="49">AVERAGE(P131:P135)</f>
+        <f t="shared" ref="P19:Q19" si="47">AVERAGE(P131:P135)</f>
         <v>3.75</v>
       </c>
       <c r="Q19" s="14">
-        <f t="shared" si="49"/>
+        <f t="shared" si="47"/>
         <v>0.75</v>
       </c>
       <c r="R19" s="15" t="e">
@@ -3333,19 +3335,19 @@
         <v>#REF!</v>
       </c>
       <c r="S19" s="14">
-        <f t="shared" ref="S19:T19" si="50">AVERAGE(S131:S135)</f>
+        <f t="shared" ref="S19:T19" si="48">AVERAGE(S131:S135)</f>
         <v>0.5</v>
       </c>
       <c r="T19" s="14">
-        <f t="shared" si="50"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="U19" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V19" s="15">
-        <f t="shared" si="8"/>
+        <f>E19/(2*(M19+0.44*S19))</f>
         <v>0.2375923970432946</v>
       </c>
       <c r="X19" s="11"/>
@@ -3358,35 +3360,35 @@
         <v>34</v>
       </c>
       <c r="E20" s="11">
-        <f t="shared" ref="E20:L20" si="51">AVERAGE(E136:E140)</f>
+        <f t="shared" ref="E20" si="49">AVERAGE(E136:E140)</f>
         <v>30.8</v>
       </c>
       <c r="F20" s="11">
-        <f t="shared" si="51"/>
+        <f>AVERAGE(F136:F140)</f>
         <v>14.6</v>
       </c>
       <c r="G20" s="11">
-        <f t="shared" si="51"/>
+        <f>AVERAGE(G136:G140)</f>
         <v>4</v>
       </c>
       <c r="H20" s="11">
-        <f t="shared" si="51"/>
+        <f>AVERAGE(H136:H140)</f>
         <v>10.6</v>
       </c>
       <c r="I20" s="11">
-        <f t="shared" si="51"/>
+        <f>AVERAGE(I136:I140)</f>
         <v>1.8</v>
       </c>
       <c r="J20" s="11">
-        <f t="shared" si="51"/>
+        <f>AVERAGE(J136:J140)</f>
         <v>0.6</v>
       </c>
       <c r="K20" s="11">
-        <f t="shared" si="51"/>
+        <f>AVERAGE(K136:K140)</f>
         <v>2.4</v>
       </c>
       <c r="L20" s="11">
-        <f t="shared" si="51"/>
+        <f>AVERAGE(L136:L140)</f>
         <v>2</v>
       </c>
       <c r="M20" s="11">
@@ -3402,11 +3404,11 @@
         <v>#REF!</v>
       </c>
       <c r="P20" s="11">
-        <f t="shared" ref="P20:Q20" si="52">AVERAGE(P136:P140)</f>
+        <f t="shared" ref="P20:Q20" si="50">AVERAGE(P136:P140)</f>
         <v>16.2</v>
       </c>
       <c r="Q20" s="11">
-        <f t="shared" si="52"/>
+        <f t="shared" si="50"/>
         <v>4</v>
       </c>
       <c r="R20" s="1" t="e">
@@ -3414,19 +3416,19 @@
         <v>#REF!</v>
       </c>
       <c r="S20" s="11">
-        <f t="shared" ref="S20:T20" si="53">AVERAGE(S136:S140)</f>
+        <f t="shared" ref="S20:T20" si="51">AVERAGE(S136:S140)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="T20" s="11">
-        <f t="shared" si="53"/>
+        <f t="shared" si="51"/>
         <v>2</v>
       </c>
       <c r="U20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.45454545454545453</v>
       </c>
       <c r="V20" s="1">
-        <f t="shared" si="8"/>
+        <f>E20/(2*(M20+0.44*S20))</f>
         <v>0.41469194312796204</v>
       </c>
       <c r="Z20" s="11"/>
@@ -3438,35 +3440,35 @@
         <v>35</v>
       </c>
       <c r="E21" s="11">
-        <f t="shared" ref="E21:L21" si="54">AVERAGE(E141:E145)</f>
+        <f t="shared" ref="E21" si="52">AVERAGE(E141:E145)</f>
         <v>10.8</v>
       </c>
       <c r="F21" s="11">
-        <f t="shared" si="54"/>
+        <f>AVERAGE(F141:F145)</f>
         <v>9.8000000000000007</v>
       </c>
       <c r="G21" s="11">
-        <f t="shared" si="54"/>
+        <f>AVERAGE(G141:G145)</f>
         <v>2.8</v>
       </c>
       <c r="H21" s="11">
-        <f t="shared" si="54"/>
+        <f>AVERAGE(H141:H145)</f>
         <v>7</v>
       </c>
       <c r="I21" s="11">
-        <f t="shared" si="54"/>
+        <f>AVERAGE(I141:I145)</f>
         <v>1.2</v>
       </c>
       <c r="J21" s="11">
-        <f t="shared" si="54"/>
+        <f>AVERAGE(J141:J145)</f>
         <v>1.2</v>
       </c>
       <c r="K21" s="11">
-        <f t="shared" si="54"/>
+        <f>AVERAGE(K141:K145)</f>
         <v>0</v>
       </c>
       <c r="L21" s="11">
-        <f t="shared" si="54"/>
+        <f>AVERAGE(L141:L145)</f>
         <v>1.4</v>
       </c>
       <c r="M21" s="11">
@@ -3482,11 +3484,11 @@
         <v>#REF!</v>
       </c>
       <c r="P21" s="11">
-        <f t="shared" ref="P21:Q21" si="55">AVERAGE(P141:P145)</f>
+        <f t="shared" ref="P21:Q21" si="53">AVERAGE(P141:P145)</f>
         <v>2.8</v>
       </c>
       <c r="Q21" s="11">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="R21" s="1" t="e">
@@ -3494,19 +3496,19 @@
         <v>#REF!</v>
       </c>
       <c r="S21" s="11">
-        <f t="shared" ref="S21:T21" si="56">AVERAGE(S141:S145)</f>
+        <f t="shared" ref="S21:T21" si="54">AVERAGE(S141:S145)</f>
         <v>3.2</v>
       </c>
       <c r="T21" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="54"/>
         <v>1.8</v>
       </c>
       <c r="U21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.5625</v>
       </c>
       <c r="V21" s="1">
-        <f t="shared" si="8"/>
+        <f>E21/(2*(M21+0.44*S21))</f>
         <v>0.32910775231594341</v>
       </c>
       <c r="Z21" s="11"/>
@@ -3518,35 +3520,35 @@
         <v>36</v>
       </c>
       <c r="E22" s="11">
-        <f t="shared" ref="E22:L22" si="57">AVERAGE(E146:E150)</f>
+        <f t="shared" ref="E22" si="55">AVERAGE(E146:E150)</f>
         <v>6</v>
       </c>
       <c r="F22" s="11">
-        <f t="shared" si="57"/>
+        <f>AVERAGE(F146:F150)</f>
         <v>9.4</v>
       </c>
       <c r="G22" s="11">
-        <f t="shared" si="57"/>
+        <f>AVERAGE(G146:G150)</f>
         <v>3.6</v>
       </c>
       <c r="H22" s="11">
-        <f t="shared" si="57"/>
+        <f>AVERAGE(H146:H150)</f>
         <v>5.8</v>
       </c>
       <c r="I22" s="11">
-        <f t="shared" si="57"/>
+        <f>AVERAGE(I146:I150)</f>
         <v>2.8</v>
       </c>
       <c r="J22" s="11">
-        <f t="shared" si="57"/>
+        <f>AVERAGE(J146:J150)</f>
         <v>0.6</v>
       </c>
       <c r="K22" s="11">
-        <f t="shared" si="57"/>
+        <f>AVERAGE(K146:K150)</f>
         <v>0.4</v>
       </c>
       <c r="L22" s="11">
-        <f t="shared" si="57"/>
+        <f>AVERAGE(L146:L150)</f>
         <v>2</v>
       </c>
       <c r="M22" s="11">
@@ -3562,11 +3564,11 @@
         <v>#REF!</v>
       </c>
       <c r="P22" s="11">
-        <f t="shared" ref="P22:Q22" si="58">AVERAGE(P146:P150)</f>
+        <f t="shared" ref="P22:Q22" si="56">AVERAGE(P146:P150)</f>
         <v>3</v>
       </c>
       <c r="Q22" s="11">
-        <f t="shared" si="58"/>
+        <f t="shared" si="56"/>
         <v>0.2</v>
       </c>
       <c r="R22" s="1" t="e">
@@ -3574,19 +3576,19 @@
         <v>#REF!</v>
       </c>
       <c r="S22" s="11">
-        <f t="shared" ref="S22:T22" si="59">AVERAGE(S146:S150)</f>
+        <f t="shared" ref="S22:T22" si="57">AVERAGE(S146:S150)</f>
         <v>3.4</v>
       </c>
       <c r="T22" s="11">
-        <f t="shared" si="59"/>
+        <f t="shared" si="57"/>
         <v>1.6</v>
       </c>
       <c r="U22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.4705882352941177</v>
       </c>
       <c r="V22" s="1">
-        <f t="shared" si="8"/>
+        <f>E22/(2*(M22+0.44*S22))</f>
         <v>0.35310734463276833</v>
       </c>
       <c r="Z22" s="11"/>
@@ -3598,35 +3600,35 @@
         <v>37</v>
       </c>
       <c r="E23" s="14">
-        <f t="shared" ref="E23:L23" si="60">AVERAGE(E151:E155)</f>
+        <f t="shared" ref="E23" si="58">AVERAGE(E151:E155)</f>
         <v>2</v>
       </c>
       <c r="F23" s="14">
-        <f t="shared" si="60"/>
+        <f>AVERAGE(F151:F155)</f>
         <v>5.8</v>
       </c>
       <c r="G23" s="14">
-        <f t="shared" si="60"/>
+        <f>AVERAGE(G151:G155)</f>
         <v>1.2</v>
       </c>
       <c r="H23" s="14">
-        <f t="shared" si="60"/>
+        <f>AVERAGE(H151:H155)</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="I23" s="14">
-        <f t="shared" si="60"/>
+        <f>AVERAGE(I151:I155)</f>
         <v>1.6</v>
       </c>
       <c r="J23" s="14">
-        <f t="shared" si="60"/>
+        <f>AVERAGE(J151:J155)</f>
         <v>1.2</v>
       </c>
       <c r="K23" s="14">
-        <f t="shared" si="60"/>
+        <f>AVERAGE(K151:K155)</f>
         <v>0.2</v>
       </c>
       <c r="L23" s="14">
-        <f t="shared" si="60"/>
+        <f>AVERAGE(L151:L155)</f>
         <v>1.4</v>
       </c>
       <c r="M23" s="14">
@@ -3642,11 +3644,11 @@
         <v>#REF!</v>
       </c>
       <c r="P23" s="14">
-        <f t="shared" ref="P23:Q23" si="61">AVERAGE(P151:P155)</f>
+        <f t="shared" ref="P23:Q23" si="59">AVERAGE(P151:P155)</f>
         <v>0.8</v>
       </c>
       <c r="Q23" s="14">
-        <f t="shared" si="61"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="R23" s="15" t="e">
@@ -3654,19 +3656,19 @@
         <v>#REF!</v>
       </c>
       <c r="S23" s="14">
-        <f t="shared" ref="S23:T23" si="62">AVERAGE(S151:S155)</f>
+        <f t="shared" ref="S23:T23" si="60">AVERAGE(S151:S155)</f>
         <v>1.4</v>
       </c>
       <c r="T23" s="14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="60"/>
         <v>0.6</v>
       </c>
       <c r="U23" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.4285714285714286</v>
       </c>
       <c r="V23" s="15">
-        <f t="shared" si="8"/>
+        <f>E23/(2*(M23+0.44*S23))</f>
         <v>0.22644927536231887</v>
       </c>
       <c r="Z23" s="11"/>
@@ -3678,35 +3680,35 @@
         <v>38</v>
       </c>
       <c r="E24" s="11">
-        <f t="shared" ref="E24:L24" si="63">AVERAGE(E156:E160)</f>
+        <f t="shared" ref="E24" si="61">AVERAGE(E156:E160)</f>
         <v>15.6</v>
       </c>
       <c r="F24" s="11">
-        <f t="shared" si="63"/>
+        <f>AVERAGE(F156:F160)</f>
         <v>10</v>
       </c>
       <c r="G24" s="11">
-        <f t="shared" si="63"/>
+        <f>AVERAGE(G156:G160)</f>
         <v>1.8</v>
       </c>
       <c r="H24" s="11">
-        <f t="shared" si="63"/>
+        <f>AVERAGE(H156:H160)</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="I24" s="11">
-        <f t="shared" si="63"/>
+        <f>AVERAGE(I156:I160)</f>
         <v>2.8</v>
       </c>
       <c r="J24" s="11">
-        <f t="shared" si="63"/>
+        <f>AVERAGE(J156:J160)</f>
         <v>1.8</v>
       </c>
       <c r="K24" s="11">
-        <f t="shared" si="63"/>
+        <f>AVERAGE(K156:K160)</f>
         <v>0.4</v>
       </c>
       <c r="L24" s="11">
-        <f t="shared" si="63"/>
+        <f>AVERAGE(L156:L160)</f>
         <v>2.6</v>
       </c>
       <c r="M24" s="11">
@@ -3722,11 +3724,11 @@
         <v>#REF!</v>
       </c>
       <c r="P24" s="11">
-        <f t="shared" ref="P24:Q24" si="64">AVERAGE(P156:P160)</f>
+        <f t="shared" ref="P24:Q24" si="62">AVERAGE(P156:P160)</f>
         <v>8.4</v>
       </c>
       <c r="Q24" s="11">
-        <f t="shared" si="64"/>
+        <f t="shared" si="62"/>
         <v>2</v>
       </c>
       <c r="R24" s="1" t="e">
@@ -3734,19 +3736,19 @@
         <v>#REF!</v>
       </c>
       <c r="S24" s="11">
-        <f t="shared" ref="S24:T24" si="65">AVERAGE(S156:S160)</f>
+        <f t="shared" ref="S24:T24" si="63">AVERAGE(S156:S160)</f>
         <v>5.8</v>
       </c>
       <c r="T24" s="11">
-        <f t="shared" si="65"/>
+        <f t="shared" si="63"/>
         <v>2.4</v>
       </c>
       <c r="U24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.41379310344827586</v>
       </c>
       <c r="V24" s="1">
-        <f t="shared" si="8"/>
+        <f>E24/(2*(M24+0.44*S24))</f>
         <v>0.39893617021276595</v>
       </c>
       <c r="Z24" s="11"/>
@@ -3758,35 +3760,35 @@
         <v>39</v>
       </c>
       <c r="E25" s="11">
-        <f t="shared" ref="E25:L25" si="66">AVERAGE(E161:E165)</f>
+        <f t="shared" ref="E25" si="64">AVERAGE(E161:E165)</f>
         <v>17.2</v>
       </c>
       <c r="F25" s="11">
-        <f t="shared" si="66"/>
+        <f>AVERAGE(F161:F165)</f>
         <v>12.4</v>
       </c>
       <c r="G25" s="11">
-        <f t="shared" si="66"/>
+        <f>AVERAGE(G161:G165)</f>
         <v>3.6</v>
       </c>
       <c r="H25" s="11">
-        <f t="shared" si="66"/>
+        <f>AVERAGE(H161:H165)</f>
         <v>8.8000000000000007</v>
       </c>
       <c r="I25" s="11">
-        <f t="shared" si="66"/>
+        <f>AVERAGE(I161:I165)</f>
         <v>2</v>
       </c>
       <c r="J25" s="11">
-        <f t="shared" si="66"/>
+        <f>AVERAGE(J161:J165)</f>
         <v>2</v>
       </c>
       <c r="K25" s="11">
-        <f t="shared" si="66"/>
+        <f>AVERAGE(K161:K165)</f>
         <v>0.4</v>
       </c>
       <c r="L25" s="11">
-        <f t="shared" si="66"/>
+        <f>AVERAGE(L161:L165)</f>
         <v>3</v>
       </c>
       <c r="M25" s="11">
@@ -3802,11 +3804,11 @@
         <v>#REF!</v>
       </c>
       <c r="P25" s="11">
-        <f t="shared" ref="P25:Q25" si="67">AVERAGE(P161:P165)</f>
+        <f t="shared" ref="P25:Q25" si="65">AVERAGE(P161:P165)</f>
         <v>4.8</v>
       </c>
       <c r="Q25" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="65"/>
         <v>0.6</v>
       </c>
       <c r="R25" s="1" t="e">
@@ -3814,19 +3816,19 @@
         <v>#REF!</v>
       </c>
       <c r="S25" s="11">
-        <f t="shared" ref="S25:T25" si="68">AVERAGE(S161:S165)</f>
+        <f t="shared" ref="S25:T25" si="66">AVERAGE(S161:S165)</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="T25" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="66"/>
         <v>1.8</v>
       </c>
       <c r="U25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="V25" s="1">
-        <f t="shared" si="8"/>
+        <f>E25/(2*(M25+0.44*S25))</f>
         <v>0.38012729844413007</v>
       </c>
       <c r="Z25" s="11"/>
@@ -3838,35 +3840,35 @@
         <v>40</v>
       </c>
       <c r="E26" s="11">
-        <f t="shared" ref="E26:L26" si="69">AVERAGE(E166:E170)</f>
+        <f t="shared" ref="E26" si="67">AVERAGE(E166:E170)</f>
         <v>8.6</v>
       </c>
       <c r="F26" s="11">
-        <f t="shared" si="69"/>
+        <f>AVERAGE(F166:F170)</f>
         <v>9</v>
       </c>
       <c r="G26" s="11">
-        <f t="shared" si="69"/>
+        <f>AVERAGE(G166:G170)</f>
         <v>3</v>
       </c>
       <c r="H26" s="11">
-        <f t="shared" si="69"/>
+        <f>AVERAGE(H166:H170)</f>
         <v>6</v>
       </c>
       <c r="I26" s="11">
-        <f t="shared" si="69"/>
+        <f>AVERAGE(I166:I170)</f>
         <v>1</v>
       </c>
       <c r="J26" s="11">
-        <f t="shared" si="69"/>
+        <f>AVERAGE(J166:J170)</f>
         <v>1.2</v>
       </c>
       <c r="K26" s="11">
-        <f t="shared" si="69"/>
+        <f>AVERAGE(K166:K170)</f>
         <v>1</v>
       </c>
       <c r="L26" s="11">
-        <f t="shared" si="69"/>
+        <f>AVERAGE(L166:L170)</f>
         <v>1.2</v>
       </c>
       <c r="M26" s="11">
@@ -3882,11 +3884,11 @@
         <v>#REF!</v>
       </c>
       <c r="P26" s="11">
-        <f t="shared" ref="P26:Q26" si="70">AVERAGE(P166:P170)</f>
+        <f t="shared" ref="P26:Q26" si="68">AVERAGE(P166:P170)</f>
         <v>2.4</v>
       </c>
       <c r="Q26" s="11">
-        <f t="shared" si="70"/>
+        <f t="shared" si="68"/>
         <v>0.4</v>
       </c>
       <c r="R26" s="1" t="e">
@@ -3894,19 +3896,19 @@
         <v>#REF!</v>
       </c>
       <c r="S26" s="11">
-        <f t="shared" ref="S26:T26" si="71">AVERAGE(S166:S170)</f>
+        <f t="shared" ref="S26:T26" si="69">AVERAGE(S166:S170)</f>
         <v>3.4</v>
       </c>
       <c r="T26" s="11">
-        <f t="shared" si="71"/>
+        <f t="shared" si="69"/>
         <v>1.4</v>
       </c>
       <c r="U26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.41176470588235292</v>
       </c>
       <c r="V26" s="1">
-        <f t="shared" si="8"/>
+        <f>E26/(2*(M26+0.44*S26))</f>
         <v>0.34970722186076769</v>
       </c>
       <c r="Z26" s="11"/>
@@ -3918,35 +3920,35 @@
         <v>41</v>
       </c>
       <c r="E27" s="14">
-        <f t="shared" ref="E27:L27" si="72">AVERAGE(E171:E175)</f>
+        <f t="shared" ref="E27" si="70">AVERAGE(E171:E175)</f>
         <v>2.6</v>
       </c>
       <c r="F27" s="14">
-        <f t="shared" si="72"/>
+        <f>AVERAGE(F171:F175)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="G27" s="14">
-        <f t="shared" si="72"/>
+        <f>AVERAGE(G171:G175)</f>
         <v>1</v>
       </c>
       <c r="H27" s="14">
-        <f t="shared" si="72"/>
+        <f>AVERAGE(H171:H175)</f>
         <v>1.2</v>
       </c>
       <c r="I27" s="14">
-        <f t="shared" si="72"/>
+        <f>AVERAGE(I171:I175)</f>
         <v>1.2</v>
       </c>
       <c r="J27" s="14">
-        <f t="shared" si="72"/>
+        <f>AVERAGE(J171:J175)</f>
         <v>0.4</v>
       </c>
       <c r="K27" s="14">
-        <f t="shared" si="72"/>
+        <f>AVERAGE(K171:K175)</f>
         <v>0.2</v>
       </c>
       <c r="L27" s="14">
-        <f t="shared" si="72"/>
+        <f>AVERAGE(L171:L175)</f>
         <v>0.2</v>
       </c>
       <c r="M27" s="14">
@@ -3962,11 +3964,11 @@
         <v>#REF!</v>
       </c>
       <c r="P27" s="14">
-        <f t="shared" ref="P27:Q27" si="73">AVERAGE(P171:P175)</f>
+        <f t="shared" ref="P27:Q27" si="71">AVERAGE(P171:P175)</f>
         <v>2.25</v>
       </c>
       <c r="Q27" s="14">
-        <f t="shared" si="73"/>
+        <f t="shared" si="71"/>
         <v>0.5</v>
       </c>
       <c r="R27" s="15" t="e">
@@ -3974,19 +3976,19 @@
         <v>#REF!</v>
       </c>
       <c r="S27" s="14">
-        <f t="shared" ref="S27:T27" si="74">AVERAGE(S171:S175)</f>
+        <f t="shared" ref="S27:T27" si="72">AVERAGE(S171:S175)</f>
         <v>1.6</v>
       </c>
       <c r="T27" s="14">
-        <f t="shared" si="74"/>
+        <f t="shared" si="72"/>
         <v>0.4</v>
       </c>
       <c r="U27" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="V27" s="15">
-        <f t="shared" si="8"/>
+        <f>E27/(2*(M27+0.44*S27))</f>
         <v>0.22592978797358362</v>
       </c>
       <c r="Z27" s="11"/>
@@ -3998,35 +4000,35 @@
         <v>42</v>
       </c>
       <c r="E28" s="11">
-        <f t="shared" ref="E28:L28" si="75">AVERAGE(E176:E180)</f>
+        <f t="shared" ref="E28" si="73">AVERAGE(E176:E180)</f>
         <v>29.6</v>
       </c>
       <c r="F28" s="11">
-        <f t="shared" si="75"/>
+        <f>AVERAGE(F176:F180)</f>
         <v>19</v>
       </c>
       <c r="G28" s="11">
-        <f t="shared" si="75"/>
+        <f>AVERAGE(G176:G180)</f>
         <v>7.8</v>
       </c>
       <c r="H28" s="11">
-        <f t="shared" si="75"/>
+        <f>AVERAGE(H176:H180)</f>
         <v>11.2</v>
       </c>
       <c r="I28" s="11">
-        <f t="shared" si="75"/>
+        <f>AVERAGE(I176:I180)</f>
         <v>3.2</v>
       </c>
       <c r="J28" s="11">
-        <f t="shared" si="75"/>
+        <f>AVERAGE(J176:J180)</f>
         <v>2.4</v>
       </c>
       <c r="K28" s="11">
-        <f t="shared" si="75"/>
+        <f>AVERAGE(K176:K180)</f>
         <v>0.4</v>
       </c>
       <c r="L28" s="11">
-        <f t="shared" si="75"/>
+        <f>AVERAGE(L176:L180)</f>
         <v>2.4</v>
       </c>
       <c r="M28" s="11">
@@ -4042,11 +4044,11 @@
         <v>#REF!</v>
       </c>
       <c r="P28" s="11">
-        <f t="shared" ref="P28:Q28" si="76">AVERAGE(P176:P180)</f>
+        <f t="shared" ref="P28:Q28" si="74">AVERAGE(P176:P180)</f>
         <v>13.2</v>
       </c>
       <c r="Q28" s="11">
-        <f t="shared" si="76"/>
+        <f t="shared" si="74"/>
         <v>2.6</v>
       </c>
       <c r="R28" s="1" t="e">
@@ -4054,19 +4056,19 @@
         <v>#REF!</v>
       </c>
       <c r="S28" s="11">
-        <f t="shared" ref="S28:T28" si="77">AVERAGE(S176:S180)</f>
+        <f t="shared" ref="S28:T28" si="75">AVERAGE(S176:S180)</f>
         <v>7.2</v>
       </c>
       <c r="T28" s="11">
-        <f t="shared" si="77"/>
+        <f t="shared" si="75"/>
         <v>2.6</v>
       </c>
       <c r="U28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.3611111111111111</v>
       </c>
       <c r="V28" s="1">
-        <f t="shared" si="8"/>
+        <f>E28/(2*(M28+0.44*S28))</f>
         <v>0.43315382814329201</v>
       </c>
       <c r="Z28" s="11"/>
@@ -4078,35 +4080,35 @@
         <v>43</v>
       </c>
       <c r="E29" s="11">
-        <f t="shared" ref="E29:L29" si="78">AVERAGE(E181:E185)</f>
+        <f t="shared" ref="E29" si="76">AVERAGE(E181:E185)</f>
         <v>16</v>
       </c>
       <c r="F29" s="11">
-        <f t="shared" si="78"/>
+        <f>AVERAGE(F181:F185)</f>
         <v>12.2</v>
       </c>
       <c r="G29" s="11">
-        <f t="shared" si="78"/>
+        <f>AVERAGE(G181:G185)</f>
         <v>4.2</v>
       </c>
       <c r="H29" s="11">
-        <f t="shared" si="78"/>
+        <f>AVERAGE(H181:H185)</f>
         <v>8</v>
       </c>
       <c r="I29" s="11">
-        <f t="shared" si="78"/>
+        <f>AVERAGE(I181:I185)</f>
         <v>1.6</v>
       </c>
       <c r="J29" s="11">
-        <f t="shared" si="78"/>
+        <f>AVERAGE(J181:J185)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="K29" s="11">
-        <f t="shared" si="78"/>
+        <f>AVERAGE(K181:K185)</f>
         <v>1</v>
       </c>
       <c r="L29" s="11">
-        <f t="shared" si="78"/>
+        <f>AVERAGE(L181:L185)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="M29" s="11">
@@ -4122,11 +4124,11 @@
         <v>#REF!</v>
       </c>
       <c r="P29" s="11">
-        <f t="shared" ref="P29:Q29" si="79">AVERAGE(P181:P185)</f>
+        <f t="shared" ref="P29:Q29" si="77">AVERAGE(P181:P185)</f>
         <v>9.6</v>
       </c>
       <c r="Q29" s="11">
-        <f t="shared" si="79"/>
+        <f t="shared" si="77"/>
         <v>2.4</v>
       </c>
       <c r="R29" s="1" t="e">
@@ -4134,19 +4136,19 @@
         <v>#REF!</v>
       </c>
       <c r="S29" s="11">
-        <f t="shared" ref="S29:T29" si="80">AVERAGE(S181:S185)</f>
+        <f t="shared" ref="S29:T29" si="78">AVERAGE(S181:S185)</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="T29" s="11">
-        <f t="shared" si="80"/>
+        <f t="shared" si="78"/>
         <v>0.8</v>
       </c>
       <c r="U29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="V29" s="1">
-        <f t="shared" si="8"/>
+        <f>E29/(2*(M29+0.44*S29))</f>
         <v>0.39666798889329635</v>
       </c>
       <c r="Z29" s="11"/>
@@ -4158,35 +4160,35 @@
         <v>44</v>
       </c>
       <c r="E30" s="11">
-        <f t="shared" ref="E30:L30" si="81">AVERAGE(E186:E190)</f>
+        <f t="shared" ref="E30" si="79">AVERAGE(E186:E190)</f>
         <v>5.8</v>
       </c>
       <c r="F30" s="11">
-        <f t="shared" si="81"/>
+        <f>AVERAGE(F186:F190)</f>
         <v>7</v>
       </c>
       <c r="G30" s="11">
-        <f t="shared" si="81"/>
+        <f>AVERAGE(G186:G190)</f>
         <v>3</v>
       </c>
       <c r="H30" s="11">
-        <f t="shared" si="81"/>
+        <f>AVERAGE(H186:H190)</f>
         <v>4</v>
       </c>
       <c r="I30" s="11">
-        <f t="shared" si="81"/>
+        <f>AVERAGE(I186:I190)</f>
         <v>2</v>
       </c>
       <c r="J30" s="11">
-        <f t="shared" si="81"/>
+        <f>AVERAGE(J186:J190)</f>
         <v>0.6</v>
       </c>
       <c r="K30" s="11">
-        <f t="shared" si="81"/>
+        <f>AVERAGE(K186:K190)</f>
         <v>0.2</v>
       </c>
       <c r="L30" s="11">
-        <f t="shared" si="81"/>
+        <f>AVERAGE(L186:L190)</f>
         <v>1.6</v>
       </c>
       <c r="M30" s="11">
@@ -4202,11 +4204,11 @@
         <v>#REF!</v>
       </c>
       <c r="P30" s="11">
-        <f t="shared" ref="P30:Q30" si="82">AVERAGE(P186:P190)</f>
+        <f t="shared" ref="P30:Q30" si="80">AVERAGE(P186:P190)</f>
         <v>3.2</v>
       </c>
       <c r="Q30" s="11">
-        <f t="shared" si="82"/>
+        <f t="shared" si="80"/>
         <v>0.8</v>
       </c>
       <c r="R30" s="1" t="e">
@@ -4214,19 +4216,19 @@
         <v>#REF!</v>
       </c>
       <c r="S30" s="11">
-        <f t="shared" ref="S30:T30" si="83">AVERAGE(S186:S190)</f>
+        <f t="shared" ref="S30:T30" si="81">AVERAGE(S186:S190)</f>
         <v>1</v>
       </c>
       <c r="T30" s="11">
-        <f t="shared" si="83"/>
+        <f t="shared" si="81"/>
         <v>0.6</v>
       </c>
       <c r="U30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="V30" s="1">
-        <f t="shared" si="8"/>
+        <f>E30/(2*(M30+0.44*S30))</f>
         <v>0.32805429864253394</v>
       </c>
       <c r="Z30" s="11"/>
@@ -4238,35 +4240,35 @@
         <v>45</v>
       </c>
       <c r="E31" s="14">
-        <f t="shared" ref="E31:L31" si="84">AVERAGE(E191:E195)</f>
+        <f t="shared" ref="E31" si="82">AVERAGE(E191:E195)</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="F31" s="14">
-        <f t="shared" si="84"/>
+        <f>AVERAGE(F191:F195)</f>
         <v>4</v>
       </c>
       <c r="G31" s="14">
-        <f t="shared" si="84"/>
+        <f>AVERAGE(G191:G195)</f>
         <v>1.2</v>
       </c>
       <c r="H31" s="14">
-        <f t="shared" si="84"/>
+        <f>AVERAGE(H191:H195)</f>
         <v>2.8</v>
       </c>
       <c r="I31" s="14">
-        <f t="shared" si="84"/>
+        <f>AVERAGE(I191:I195)</f>
         <v>1.4</v>
       </c>
       <c r="J31" s="14">
-        <f t="shared" si="84"/>
+        <f>AVERAGE(J191:J195)</f>
         <v>0.6</v>
       </c>
       <c r="K31" s="14">
-        <f t="shared" si="84"/>
+        <f>AVERAGE(K191:K195)</f>
         <v>0</v>
       </c>
       <c r="L31" s="14">
-        <f t="shared" si="84"/>
+        <f>AVERAGE(L191:L195)</f>
         <v>0.6</v>
       </c>
       <c r="M31" s="14">
@@ -4282,11 +4284,11 @@
         <v>#REF!</v>
       </c>
       <c r="P31" s="14">
-        <f t="shared" ref="P31:Q31" si="85">AVERAGE(P191:P195)</f>
+        <f t="shared" ref="P31:Q31" si="83">AVERAGE(P191:P195)</f>
         <v>4.2</v>
       </c>
       <c r="Q31" s="14">
-        <f t="shared" si="85"/>
+        <f t="shared" si="83"/>
         <v>1.4</v>
       </c>
       <c r="R31" s="15" t="e">
@@ -4294,19 +4296,19 @@
         <v>#REF!</v>
       </c>
       <c r="S31" s="14">
-        <f t="shared" ref="S31:T31" si="86">AVERAGE(S191:S195)</f>
+        <f t="shared" ref="S31:T31" si="84">AVERAGE(S191:S195)</f>
         <v>0</v>
       </c>
       <c r="T31" s="14">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="U31" s="15" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V31" s="15">
-        <f t="shared" si="8"/>
+        <f>E31/(2*(M31+0.44*S31))</f>
         <v>0.33823529411764702</v>
       </c>
     </row>
@@ -4315,35 +4317,35 @@
         <v>46</v>
       </c>
       <c r="E32" s="11">
-        <f t="shared" ref="E32:L32" si="87">AVERAGE(E196:E200)</f>
+        <f t="shared" ref="E32" si="85">AVERAGE(E196:E200)</f>
         <v>27.5</v>
       </c>
       <c r="F32" s="11">
-        <f t="shared" si="87"/>
+        <f>AVERAGE(F196:F200)</f>
         <v>16.25</v>
       </c>
       <c r="G32" s="11">
-        <f t="shared" si="87"/>
+        <f>AVERAGE(G196:G200)</f>
         <v>4.25</v>
       </c>
       <c r="H32" s="11">
-        <f t="shared" si="87"/>
+        <f>AVERAGE(H196:H200)</f>
         <v>12</v>
       </c>
       <c r="I32" s="11">
-        <f t="shared" si="87"/>
+        <f>AVERAGE(I196:I200)</f>
         <v>3</v>
       </c>
       <c r="J32" s="11">
-        <f t="shared" si="87"/>
+        <f>AVERAGE(J196:J200)</f>
         <v>2</v>
       </c>
       <c r="K32" s="11">
-        <f t="shared" si="87"/>
+        <f>AVERAGE(K196:K200)</f>
         <v>1.5</v>
       </c>
       <c r="L32" s="11">
-        <f t="shared" si="87"/>
+        <f>AVERAGE(L196:L200)</f>
         <v>1.25</v>
       </c>
       <c r="M32" s="11">
@@ -4359,11 +4361,11 @@
         <v>#REF!</v>
       </c>
       <c r="P32" s="11">
-        <f t="shared" ref="P32:Q32" si="88">AVERAGE(P196:P200)</f>
+        <f t="shared" ref="P32:Q32" si="86">AVERAGE(P196:P200)</f>
         <v>11</v>
       </c>
       <c r="Q32" s="11">
-        <f t="shared" si="88"/>
+        <f t="shared" si="86"/>
         <v>2.25</v>
       </c>
       <c r="R32" s="1" t="e">
@@ -4371,19 +4373,19 @@
         <v>#REF!</v>
       </c>
       <c r="S32" s="11">
-        <f t="shared" ref="S32:T32" si="89">AVERAGE(S196:S200)</f>
+        <f t="shared" ref="S32:T32" si="87">AVERAGE(S196:S200)</f>
         <v>6.25</v>
       </c>
       <c r="T32" s="11">
-        <f t="shared" si="89"/>
+        <f t="shared" si="87"/>
         <v>4.25</v>
       </c>
       <c r="U32" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.68</v>
       </c>
       <c r="V32" s="1">
-        <f t="shared" si="8"/>
+        <f>E32/(2*(M32+0.44*S32))</f>
         <v>0.50458715596330272</v>
       </c>
     </row>
@@ -4392,35 +4394,35 @@
         <v>47</v>
       </c>
       <c r="E33" s="11">
-        <f t="shared" ref="E33:L33" si="90">AVERAGE(E201:E205)</f>
+        <f t="shared" ref="E33" si="88">AVERAGE(E201:E205)</f>
         <v>12.8</v>
       </c>
       <c r="F33" s="11">
-        <f t="shared" si="90"/>
+        <f>AVERAGE(F201:F205)</f>
         <v>10.4</v>
       </c>
       <c r="G33" s="11">
-        <f t="shared" si="90"/>
+        <f>AVERAGE(G201:G205)</f>
         <v>3.2</v>
       </c>
       <c r="H33" s="11">
-        <f t="shared" si="90"/>
+        <f>AVERAGE(H201:H205)</f>
         <v>7.2</v>
       </c>
       <c r="I33" s="11">
-        <f t="shared" si="90"/>
+        <f>AVERAGE(I201:I205)</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="J33" s="11">
-        <f t="shared" si="90"/>
+        <f>AVERAGE(J201:J205)</f>
         <v>0.8</v>
       </c>
       <c r="K33" s="11">
-        <f t="shared" si="90"/>
+        <f>AVERAGE(K201:K205)</f>
         <v>0.4</v>
       </c>
       <c r="L33" s="11">
-        <f t="shared" si="90"/>
+        <f>AVERAGE(L201:L205)</f>
         <v>3.8</v>
       </c>
       <c r="M33" s="11">
@@ -4436,11 +4438,11 @@
         <v>#REF!</v>
       </c>
       <c r="P33" s="11">
-        <f t="shared" ref="P33:Q33" si="91">AVERAGE(P201:P205)</f>
+        <f t="shared" ref="P33:Q33" si="89">AVERAGE(P201:P205)</f>
         <v>0.2</v>
       </c>
       <c r="Q33" s="11">
-        <f t="shared" si="91"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="R33" s="1" t="e">
@@ -4448,19 +4450,19 @@
         <v>#REF!</v>
       </c>
       <c r="S33" s="11">
-        <f t="shared" ref="S33:T33" si="92">AVERAGE(S201:S205)</f>
+        <f t="shared" ref="S33:T33" si="90">AVERAGE(S201:S205)</f>
         <v>4.8</v>
       </c>
       <c r="T33" s="11">
-        <f t="shared" si="92"/>
+        <f t="shared" si="90"/>
         <v>2.4</v>
       </c>
       <c r="U33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="V33" s="1">
-        <f t="shared" si="8"/>
+        <f>E33/(2*(M33+0.44*S33))</f>
         <v>0.41258380608561118</v>
       </c>
     </row>
@@ -4469,35 +4471,35 @@
         <v>48</v>
       </c>
       <c r="E34" s="11">
-        <f t="shared" ref="E34:L34" si="93">AVERAGE(E206:E210)</f>
+        <f t="shared" ref="E34" si="91">AVERAGE(E206:E210)</f>
         <v>14.2</v>
       </c>
       <c r="F34" s="11">
-        <f t="shared" si="93"/>
+        <f>AVERAGE(F206:F210)</f>
         <v>5.8</v>
       </c>
       <c r="G34" s="11">
-        <f t="shared" si="93"/>
+        <f>AVERAGE(G206:G210)</f>
         <v>1.4</v>
       </c>
       <c r="H34" s="11">
-        <f t="shared" si="93"/>
+        <f>AVERAGE(H206:H210)</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="I34" s="11">
-        <f t="shared" si="93"/>
+        <f>AVERAGE(I206:I210)</f>
         <v>1.8</v>
       </c>
       <c r="J34" s="11">
-        <f t="shared" si="93"/>
+        <f>AVERAGE(J206:J210)</f>
         <v>1</v>
       </c>
       <c r="K34" s="11">
-        <f t="shared" si="93"/>
+        <f>AVERAGE(K206:K210)</f>
         <v>0.4</v>
       </c>
       <c r="L34" s="11">
-        <f t="shared" si="93"/>
+        <f>AVERAGE(L206:L210)</f>
         <v>1.8</v>
       </c>
       <c r="M34" s="11">
@@ -4513,11 +4515,11 @@
         <v>#REF!</v>
       </c>
       <c r="P34" s="11">
-        <f t="shared" ref="P34:Q34" si="94">AVERAGE(P206:P210)</f>
+        <f t="shared" ref="P34:Q34" si="92">AVERAGE(P206:P210)</f>
         <v>2.4</v>
       </c>
       <c r="Q34" s="11">
-        <f t="shared" si="94"/>
+        <f t="shared" si="92"/>
         <v>0.4</v>
       </c>
       <c r="R34" s="1" t="e">
@@ -4525,19 +4527,19 @@
         <v>#REF!</v>
       </c>
       <c r="S34" s="11">
-        <f t="shared" ref="S34:T34" si="95">AVERAGE(S206:S210)</f>
+        <f t="shared" ref="S34:T34" si="93">AVERAGE(S206:S210)</f>
         <v>2</v>
       </c>
       <c r="T34" s="11">
-        <f t="shared" si="95"/>
+        <f t="shared" si="93"/>
         <v>1.2</v>
       </c>
       <c r="U34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
       <c r="V34" s="1">
-        <f t="shared" si="8"/>
+        <f>E34/(2*(M34+0.44*S34))</f>
         <v>0.41569086651053866</v>
       </c>
     </row>
@@ -4546,35 +4548,35 @@
         <v>49</v>
       </c>
       <c r="E35" s="11">
-        <f t="shared" ref="E35:L35" si="96">AVERAGE(E211:E215)</f>
+        <f t="shared" ref="E35" si="94">AVERAGE(E211:E215)</f>
         <v>3.4</v>
       </c>
       <c r="F35" s="11">
-        <f t="shared" si="96"/>
+        <f>AVERAGE(F211:F215)</f>
         <v>3</v>
       </c>
       <c r="G35" s="11">
-        <f t="shared" si="96"/>
+        <f>AVERAGE(G211:G215)</f>
         <v>1</v>
       </c>
       <c r="H35" s="11">
-        <f t="shared" si="96"/>
+        <f>AVERAGE(H211:H215)</f>
         <v>2</v>
       </c>
       <c r="I35" s="11">
-        <f t="shared" si="96"/>
+        <f>AVERAGE(I211:I215)</f>
         <v>1.8</v>
       </c>
       <c r="J35" s="11">
-        <f t="shared" si="96"/>
+        <f>AVERAGE(J211:J215)</f>
         <v>0.6</v>
       </c>
       <c r="K35" s="11">
-        <f t="shared" si="96"/>
+        <f>AVERAGE(K211:K215)</f>
         <v>0</v>
       </c>
       <c r="L35" s="11">
-        <f t="shared" si="96"/>
+        <f>AVERAGE(L211:L215)</f>
         <v>0.6</v>
       </c>
       <c r="M35" s="11">
@@ -4590,11 +4592,11 @@
         <v>#REF!</v>
       </c>
       <c r="P35" s="11">
-        <f t="shared" ref="P35:Q35" si="97">AVERAGE(P211:P215)</f>
+        <f t="shared" ref="P35:Q35" si="95">AVERAGE(P211:P215)</f>
         <v>0.2</v>
       </c>
       <c r="Q35" s="11">
-        <f t="shared" si="97"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="R35" s="1" t="e">
@@ -4602,19 +4604,19 @@
         <v>#REF!</v>
       </c>
       <c r="S35" s="11">
-        <f t="shared" ref="S35:T35" si="98">AVERAGE(S211:S215)</f>
+        <f t="shared" ref="S35:T35" si="96">AVERAGE(S211:S215)</f>
         <v>0.2</v>
       </c>
       <c r="T35" s="11">
-        <f t="shared" si="98"/>
+        <f t="shared" si="96"/>
         <v>0.2</v>
       </c>
       <c r="U35" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="V35" s="1">
-        <f t="shared" si="8"/>
+        <f>E35/(2*(M35+0.44*S35))</f>
         <v>0.63244047619047616</v>
       </c>
       <c r="Y35" s="79" t="s">
@@ -4774,78 +4776,78 @@
     </row>
     <row r="40" spans="4:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D40" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E40" s="37">
-        <f t="shared" ref="E40:N40" si="99">SUM(E4:E7)</f>
+        <f t="shared" ref="E40:N40" si="97">SUM(E4:E7)</f>
         <v>44.199999999999996</v>
       </c>
       <c r="F40" s="37">
+        <f t="shared" si="97"/>
+        <v>37.200000000000003</v>
+      </c>
+      <c r="G40" s="37">
+        <f t="shared" si="97"/>
+        <v>8</v>
+      </c>
+      <c r="H40" s="37">
+        <f t="shared" si="97"/>
+        <v>29.2</v>
+      </c>
+      <c r="I40" s="37">
+        <f t="shared" si="97"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J40" s="37">
+        <f t="shared" si="97"/>
+        <v>3.4</v>
+      </c>
+      <c r="K40" s="37">
+        <f t="shared" si="97"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L40" s="37">
+        <f t="shared" si="97"/>
+        <v>8</v>
+      </c>
+      <c r="M40" s="37">
+        <f t="shared" si="97"/>
+        <v>55.2</v>
+      </c>
+      <c r="N40" s="37">
+        <f t="shared" si="97"/>
+        <v>17.8</v>
+      </c>
+      <c r="O40" s="38">
+        <f t="shared" ref="O40:O47" si="98">N40/M40</f>
+        <v>0.32246376811594202</v>
+      </c>
+      <c r="P40" s="37">
+        <f t="shared" ref="P40:Q40" si="99">SUM(P4:P7)</f>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="Q40" s="37">
         <f t="shared" si="99"/>
-        <v>37.200000000000003</v>
-      </c>
-      <c r="G40" s="37">
-        <f t="shared" si="99"/>
-        <v>8</v>
-      </c>
-      <c r="H40" s="37">
-        <f t="shared" si="99"/>
-        <v>29.2</v>
-      </c>
-      <c r="I40" s="37">
-        <f t="shared" si="99"/>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="J40" s="37">
-        <f t="shared" si="99"/>
-        <v>3.4</v>
-      </c>
-      <c r="K40" s="37">
-        <f t="shared" si="99"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L40" s="37">
-        <f t="shared" si="99"/>
-        <v>8</v>
-      </c>
-      <c r="M40" s="37">
-        <f t="shared" si="99"/>
-        <v>55.2</v>
-      </c>
-      <c r="N40" s="37">
-        <f t="shared" si="99"/>
-        <v>17.8</v>
-      </c>
-      <c r="O40" s="38">
-        <f t="shared" ref="O40:O47" si="100">N40/M40</f>
-        <v>0.32246376811594202</v>
-      </c>
-      <c r="P40" s="37">
-        <f t="shared" ref="P40:Q40" si="101">SUM(P4:P7)</f>
-        <v>18.600000000000001</v>
-      </c>
-      <c r="Q40" s="37">
+        <v>4.8</v>
+      </c>
+      <c r="R40" s="38">
+        <f t="shared" ref="R40:R47" si="100">Q40/P40</f>
+        <v>0.25806451612903225</v>
+      </c>
+      <c r="S40" s="37">
+        <f t="shared" ref="S40:T40" si="101">SUM(S4:S7)</f>
+        <v>9</v>
+      </c>
+      <c r="T40" s="37">
         <f t="shared" si="101"/>
-        <v>4.8</v>
-      </c>
-      <c r="R40" s="38">
-        <f t="shared" ref="R40:R47" si="102">Q40/P40</f>
-        <v>0.25806451612903225</v>
-      </c>
-      <c r="S40" s="37">
-        <f t="shared" ref="S40:T40" si="103">SUM(S4:S7)</f>
-        <v>9</v>
-      </c>
-      <c r="T40" s="37">
-        <f t="shared" si="103"/>
         <v>3.4000000000000004</v>
       </c>
       <c r="U40" s="38">
-        <f t="shared" ref="U40:U47" si="104">T40/S40</f>
+        <f t="shared" ref="U40:U47" si="102">T40/S40</f>
         <v>0.37777777777777782</v>
       </c>
       <c r="V40" s="39">
-        <f t="shared" ref="V40:V47" si="105">AVERAGE(Z40,AB40,AD40,AF40,AH40,AJ40)</f>
+        <f t="shared" ref="V40:V47" si="103">AVERAGE(Z40,AB40,AD40,AF40,AH40,AJ40)</f>
         <v>51.8</v>
       </c>
       <c r="Y40" s="12" t="s">
@@ -4890,75 +4892,75 @@
         <v>66</v>
       </c>
       <c r="E41" s="37">
-        <f t="shared" ref="E41:N41" si="106">SUM(E8:E11)</f>
+        <f t="shared" ref="E41:N41" si="104">SUM(E8:E11)</f>
         <v>50.4</v>
       </c>
       <c r="F41" s="37">
+        <f t="shared" si="104"/>
+        <v>29.6</v>
+      </c>
+      <c r="G41" s="37">
+        <f t="shared" si="104"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H41" s="37">
+        <f t="shared" si="104"/>
+        <v>20.799999999999997</v>
+      </c>
+      <c r="I41" s="37">
+        <f t="shared" si="104"/>
+        <v>8.4</v>
+      </c>
+      <c r="J41" s="37">
+        <f t="shared" si="104"/>
+        <v>3</v>
+      </c>
+      <c r="K41" s="37">
+        <f t="shared" si="104"/>
+        <v>2.4</v>
+      </c>
+      <c r="L41" s="37">
+        <f t="shared" si="104"/>
+        <v>5.4</v>
+      </c>
+      <c r="M41" s="37">
+        <f t="shared" si="104"/>
+        <v>56.6</v>
+      </c>
+      <c r="N41" s="37">
+        <f t="shared" si="104"/>
+        <v>19.199999999999996</v>
+      </c>
+      <c r="O41" s="38">
+        <f t="shared" si="98"/>
+        <v>0.33922261484098931</v>
+      </c>
+      <c r="P41" s="37">
+        <f t="shared" ref="P41:Q41" si="105">SUM(P8:P11)</f>
+        <v>22.999999999999996</v>
+      </c>
+      <c r="Q41" s="37">
+        <f t="shared" si="105"/>
+        <v>5.6</v>
+      </c>
+      <c r="R41" s="38">
+        <f t="shared" si="100"/>
+        <v>0.24347826086956523</v>
+      </c>
+      <c r="S41" s="37">
+        <f t="shared" ref="S41:T41" si="106">SUM(S8:S11)</f>
+        <v>11.6</v>
+      </c>
+      <c r="T41" s="37">
         <f t="shared" si="106"/>
-        <v>29.6</v>
-      </c>
-      <c r="G41" s="37">
-        <f t="shared" si="106"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="H41" s="37">
-        <f t="shared" si="106"/>
-        <v>20.799999999999997</v>
-      </c>
-      <c r="I41" s="37">
-        <f t="shared" si="106"/>
-        <v>8.4</v>
-      </c>
-      <c r="J41" s="37">
-        <f t="shared" si="106"/>
-        <v>3</v>
-      </c>
-      <c r="K41" s="37">
-        <f t="shared" si="106"/>
-        <v>2.4</v>
-      </c>
-      <c r="L41" s="37">
-        <f t="shared" si="106"/>
-        <v>5.4</v>
-      </c>
-      <c r="M41" s="37">
-        <f t="shared" si="106"/>
-        <v>56.6</v>
-      </c>
-      <c r="N41" s="37">
-        <f t="shared" si="106"/>
-        <v>19.199999999999996</v>
-      </c>
-      <c r="O41" s="38">
-        <f t="shared" si="100"/>
-        <v>0.33922261484098931</v>
-      </c>
-      <c r="P41" s="37">
-        <f t="shared" ref="P41:Q41" si="107">SUM(P8:P11)</f>
-        <v>22.999999999999996</v>
-      </c>
-      <c r="Q41" s="37">
-        <f t="shared" si="107"/>
-        <v>5.6</v>
-      </c>
-      <c r="R41" s="38">
+        <v>6.1999999999999993</v>
+      </c>
+      <c r="U41" s="38">
         <f t="shared" si="102"/>
-        <v>0.24347826086956523</v>
-      </c>
-      <c r="S41" s="37">
-        <f t="shared" ref="S41:T41" si="108">SUM(S8:S11)</f>
-        <v>11.6</v>
-      </c>
-      <c r="T41" s="37">
-        <f t="shared" si="108"/>
-        <v>6.1999999999999993</v>
-      </c>
-      <c r="U41" s="38">
-        <f t="shared" si="104"/>
         <v>0.53448275862068961</v>
       </c>
       <c r="V41" s="39">
-        <f t="shared" si="105"/>
+        <f t="shared" si="103"/>
         <v>56.4</v>
       </c>
       <c r="Y41" s="17" t="s">
@@ -5003,75 +5005,75 @@
         <v>62</v>
       </c>
       <c r="E42" s="37">
-        <f t="shared" ref="E42:N42" si="109">SUM(E12:E15)</f>
+        <f t="shared" ref="E42:N42" si="107">SUM(E12:E15)</f>
         <v>49.600000000000009</v>
       </c>
       <c r="F42" s="37">
+        <f t="shared" si="107"/>
+        <v>33.200000000000003</v>
+      </c>
+      <c r="G42" s="37">
+        <f t="shared" si="107"/>
+        <v>8</v>
+      </c>
+      <c r="H42" s="37">
+        <f t="shared" si="107"/>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="I42" s="37">
+        <f t="shared" si="107"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J42" s="37">
+        <f t="shared" si="107"/>
+        <v>3.8</v>
+      </c>
+      <c r="K42" s="37">
+        <f t="shared" si="107"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L42" s="37">
+        <f t="shared" si="107"/>
+        <v>6</v>
+      </c>
+      <c r="M42" s="37">
+        <f t="shared" si="107"/>
+        <v>60.8</v>
+      </c>
+      <c r="N42" s="37">
+        <f t="shared" si="107"/>
+        <v>19.2</v>
+      </c>
+      <c r="O42" s="38">
+        <f t="shared" si="98"/>
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="P42" s="37">
+        <f t="shared" ref="P42:Q42" si="108">SUM(P12:P15)</f>
+        <v>30.2</v>
+      </c>
+      <c r="Q42" s="37">
+        <f t="shared" si="108"/>
+        <v>6</v>
+      </c>
+      <c r="R42" s="38">
+        <f t="shared" si="100"/>
+        <v>0.19867549668874174</v>
+      </c>
+      <c r="S42" s="37">
+        <f t="shared" ref="S42:T42" si="109">SUM(S12:S15)</f>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="T42" s="37">
         <f t="shared" si="109"/>
-        <v>33.200000000000003</v>
-      </c>
-      <c r="G42" s="37">
-        <f t="shared" si="109"/>
-        <v>8</v>
-      </c>
-      <c r="H42" s="37">
-        <f t="shared" si="109"/>
-        <v>25.200000000000003</v>
-      </c>
-      <c r="I42" s="37">
-        <f t="shared" si="109"/>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="J42" s="37">
-        <f t="shared" si="109"/>
-        <v>3.8</v>
-      </c>
-      <c r="K42" s="37">
-        <f t="shared" si="109"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L42" s="37">
-        <f t="shared" si="109"/>
-        <v>6</v>
-      </c>
-      <c r="M42" s="37">
-        <f t="shared" si="109"/>
-        <v>60.8</v>
-      </c>
-      <c r="N42" s="37">
-        <f t="shared" si="109"/>
-        <v>19.2</v>
-      </c>
-      <c r="O42" s="38">
-        <f t="shared" si="100"/>
-        <v>0.31578947368421051</v>
-      </c>
-      <c r="P42" s="37">
-        <f t="shared" ref="P42:Q42" si="110">SUM(P12:P15)</f>
-        <v>30.2</v>
-      </c>
-      <c r="Q42" s="37">
-        <f t="shared" si="110"/>
-        <v>6</v>
-      </c>
-      <c r="R42" s="38">
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="U42" s="38">
         <f t="shared" si="102"/>
-        <v>0.19867549668874174</v>
-      </c>
-      <c r="S42" s="37">
-        <f t="shared" ref="S42:T42" si="111">SUM(S12:S15)</f>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="T42" s="37">
-        <f t="shared" si="111"/>
-        <v>5.3999999999999995</v>
-      </c>
-      <c r="U42" s="38">
-        <f t="shared" si="104"/>
         <v>0.61363636363636354</v>
       </c>
       <c r="V42" s="39">
-        <f t="shared" si="105"/>
+        <f t="shared" si="103"/>
         <v>48.6</v>
       </c>
       <c r="Y42" s="19" t="s">
@@ -5116,75 +5118,75 @@
         <v>63</v>
       </c>
       <c r="E43" s="37">
-        <f t="shared" ref="E43:N43" si="112">SUM(E16:E19)</f>
+        <f t="shared" ref="E43:N43" si="110">SUM(E16:E19)</f>
         <v>47.9</v>
       </c>
       <c r="F43" s="37">
+        <f t="shared" si="110"/>
+        <v>36.450000000000003</v>
+      </c>
+      <c r="G43" s="37">
+        <f t="shared" si="110"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H43" s="37">
+        <f t="shared" si="110"/>
+        <v>28.15</v>
+      </c>
+      <c r="I43" s="37">
+        <f t="shared" si="110"/>
+        <v>9</v>
+      </c>
+      <c r="J43" s="37">
+        <f t="shared" si="110"/>
+        <v>5.95</v>
+      </c>
+      <c r="K43" s="37">
+        <f t="shared" si="110"/>
+        <v>4.25</v>
+      </c>
+      <c r="L43" s="37">
+        <f t="shared" si="110"/>
+        <v>10.35</v>
+      </c>
+      <c r="M43" s="37">
+        <f t="shared" si="110"/>
+        <v>59.900000000000006</v>
+      </c>
+      <c r="N43" s="37">
+        <f t="shared" si="110"/>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="O43" s="38">
+        <f t="shared" si="98"/>
+        <v>0.3238731218697829</v>
+      </c>
+      <c r="P43" s="37">
+        <f t="shared" ref="P43:Q43" si="111">SUM(P16:P19)</f>
+        <v>17.149999999999999</v>
+      </c>
+      <c r="Q43" s="37">
+        <f t="shared" si="111"/>
+        <v>3.55</v>
+      </c>
+      <c r="R43" s="38">
+        <f t="shared" si="100"/>
+        <v>0.20699708454810498</v>
+      </c>
+      <c r="S43" s="37">
+        <f t="shared" ref="S43:T43" si="112">SUM(S16:S19)</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="T43" s="37">
         <f t="shared" si="112"/>
-        <v>36.450000000000003</v>
-      </c>
-      <c r="G43" s="37">
-        <f t="shared" si="112"/>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="H43" s="37">
-        <f t="shared" si="112"/>
-        <v>28.15</v>
-      </c>
-      <c r="I43" s="37">
-        <f t="shared" si="112"/>
-        <v>9</v>
-      </c>
-      <c r="J43" s="37">
-        <f t="shared" si="112"/>
-        <v>5.95</v>
-      </c>
-      <c r="K43" s="37">
-        <f t="shared" si="112"/>
-        <v>4.25</v>
-      </c>
-      <c r="L43" s="37">
-        <f t="shared" si="112"/>
-        <v>10.35</v>
-      </c>
-      <c r="M43" s="37">
-        <f t="shared" si="112"/>
-        <v>59.900000000000006</v>
-      </c>
-      <c r="N43" s="37">
-        <f t="shared" si="112"/>
-        <v>19.399999999999999</v>
-      </c>
-      <c r="O43" s="38">
-        <f t="shared" si="100"/>
-        <v>0.3238731218697829</v>
-      </c>
-      <c r="P43" s="37">
-        <f t="shared" ref="P43:Q43" si="113">SUM(P16:P19)</f>
-        <v>17.149999999999999</v>
-      </c>
-      <c r="Q43" s="37">
-        <f t="shared" si="113"/>
-        <v>3.55</v>
-      </c>
-      <c r="R43" s="38">
+        <v>5.8</v>
+      </c>
+      <c r="U43" s="38">
         <f t="shared" si="102"/>
-        <v>0.20699708454810498</v>
-      </c>
-      <c r="S43" s="37">
-        <f t="shared" ref="S43:T43" si="114">SUM(S16:S19)</f>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="T43" s="37">
-        <f t="shared" si="114"/>
-        <v>5.8</v>
-      </c>
-      <c r="U43" s="38">
-        <f t="shared" si="104"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="V43" s="39">
-        <f t="shared" si="105"/>
+        <f t="shared" si="103"/>
         <v>50.2</v>
       </c>
       <c r="Y43" s="40" t="s">
@@ -5228,75 +5230,75 @@
         <v>61</v>
       </c>
       <c r="E44" s="37">
-        <f t="shared" ref="E44:N44" si="115">SUM(E20:E23)</f>
+        <f t="shared" ref="E44:N44" si="113">SUM(E20:E23)</f>
         <v>49.6</v>
       </c>
       <c r="F44" s="37">
+        <f t="shared" si="113"/>
+        <v>39.599999999999994</v>
+      </c>
+      <c r="G44" s="37">
+        <f t="shared" si="113"/>
+        <v>11.6</v>
+      </c>
+      <c r="H44" s="37">
+        <f t="shared" si="113"/>
+        <v>28</v>
+      </c>
+      <c r="I44" s="37">
+        <f t="shared" si="113"/>
+        <v>7.4</v>
+      </c>
+      <c r="J44" s="37">
+        <f t="shared" si="113"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="K44" s="37">
+        <f t="shared" si="113"/>
+        <v>3</v>
+      </c>
+      <c r="L44" s="37">
+        <f t="shared" si="113"/>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="M44" s="37">
+        <f t="shared" si="113"/>
+        <v>61</v>
+      </c>
+      <c r="N44" s="37">
+        <f t="shared" si="113"/>
+        <v>20</v>
+      </c>
+      <c r="O44" s="38">
+        <f t="shared" si="98"/>
+        <v>0.32786885245901637</v>
+      </c>
+      <c r="P44" s="37">
+        <f t="shared" ref="P44:Q44" si="114">SUM(P20:P23)</f>
+        <v>22.8</v>
+      </c>
+      <c r="Q44" s="37">
+        <f t="shared" si="114"/>
+        <v>4.2</v>
+      </c>
+      <c r="R44" s="38">
+        <f t="shared" si="100"/>
+        <v>0.18421052631578946</v>
+      </c>
+      <c r="S44" s="37">
+        <f t="shared" ref="S44:T44" si="115">SUM(S20:S23)</f>
+        <v>12.4</v>
+      </c>
+      <c r="T44" s="37">
         <f t="shared" si="115"/>
-        <v>39.599999999999994</v>
-      </c>
-      <c r="G44" s="37">
-        <f t="shared" si="115"/>
-        <v>11.6</v>
-      </c>
-      <c r="H44" s="37">
-        <f t="shared" si="115"/>
-        <v>28</v>
-      </c>
-      <c r="I44" s="37">
-        <f t="shared" si="115"/>
-        <v>7.4</v>
-      </c>
-      <c r="J44" s="37">
-        <f t="shared" si="115"/>
-        <v>3.5999999999999996</v>
-      </c>
-      <c r="K44" s="37">
-        <f t="shared" si="115"/>
-        <v>3</v>
-      </c>
-      <c r="L44" s="37">
-        <f t="shared" si="115"/>
-        <v>6.8000000000000007</v>
-      </c>
-      <c r="M44" s="37">
-        <f t="shared" si="115"/>
-        <v>61</v>
-      </c>
-      <c r="N44" s="37">
-        <f t="shared" si="115"/>
-        <v>20</v>
-      </c>
-      <c r="O44" s="38">
-        <f t="shared" si="100"/>
-        <v>0.32786885245901637</v>
-      </c>
-      <c r="P44" s="37">
-        <f t="shared" ref="P44:Q44" si="116">SUM(P20:P23)</f>
-        <v>22.8</v>
-      </c>
-      <c r="Q44" s="37">
-        <f t="shared" si="116"/>
-        <v>4.2</v>
-      </c>
-      <c r="R44" s="38">
+        <v>6</v>
+      </c>
+      <c r="U44" s="38">
         <f t="shared" si="102"/>
-        <v>0.18421052631578946</v>
-      </c>
-      <c r="S44" s="37">
-        <f t="shared" ref="S44:T44" si="117">SUM(S20:S23)</f>
-        <v>12.4</v>
-      </c>
-      <c r="T44" s="37">
-        <f t="shared" si="117"/>
-        <v>6</v>
-      </c>
-      <c r="U44" s="38">
-        <f t="shared" si="104"/>
         <v>0.48387096774193544</v>
       </c>
       <c r="V44" s="39">
-        <f t="shared" si="105"/>
+        <f t="shared" si="103"/>
         <v>51.2</v>
       </c>
       <c r="Y44" s="24" t="s">
@@ -5341,75 +5343,75 @@
         <v>64</v>
       </c>
       <c r="E45" s="37">
-        <f t="shared" ref="E45:N45" si="118">SUM(E24:E27)</f>
+        <f t="shared" ref="E45:N45" si="116">SUM(E24:E27)</f>
         <v>44</v>
       </c>
       <c r="F45" s="37">
+        <f t="shared" si="116"/>
+        <v>33.6</v>
+      </c>
+      <c r="G45" s="37">
+        <f t="shared" si="116"/>
+        <v>9.4</v>
+      </c>
+      <c r="H45" s="37">
+        <f t="shared" si="116"/>
+        <v>24.2</v>
+      </c>
+      <c r="I45" s="37">
+        <f t="shared" si="116"/>
+        <v>7</v>
+      </c>
+      <c r="J45" s="37">
+        <f t="shared" si="116"/>
+        <v>5.4</v>
+      </c>
+      <c r="K45" s="37">
+        <f t="shared" si="116"/>
+        <v>2</v>
+      </c>
+      <c r="L45" s="37">
+        <f t="shared" si="116"/>
+        <v>7</v>
+      </c>
+      <c r="M45" s="37">
+        <f t="shared" si="116"/>
+        <v>53.45</v>
+      </c>
+      <c r="N45" s="37">
+        <f t="shared" si="116"/>
+        <v>17.5</v>
+      </c>
+      <c r="O45" s="38">
+        <f t="shared" si="98"/>
+        <v>0.32740879326473338</v>
+      </c>
+      <c r="P45" s="37">
+        <f t="shared" ref="P45:Q45" si="117">SUM(P24:P27)</f>
+        <v>17.850000000000001</v>
+      </c>
+      <c r="Q45" s="37">
+        <f t="shared" si="117"/>
+        <v>3.5</v>
+      </c>
+      <c r="R45" s="38">
+        <f t="shared" si="100"/>
+        <v>0.19607843137254902</v>
+      </c>
+      <c r="S45" s="37">
+        <f t="shared" ref="S45:T45" si="118">SUM(S24:S27)</f>
+        <v>15.399999999999999</v>
+      </c>
+      <c r="T45" s="37">
         <f t="shared" si="118"/>
-        <v>33.6</v>
-      </c>
-      <c r="G45" s="37">
-        <f t="shared" si="118"/>
-        <v>9.4</v>
-      </c>
-      <c r="H45" s="37">
-        <f t="shared" si="118"/>
-        <v>24.2</v>
-      </c>
-      <c r="I45" s="37">
-        <f t="shared" si="118"/>
-        <v>7</v>
-      </c>
-      <c r="J45" s="37">
-        <f t="shared" si="118"/>
-        <v>5.4</v>
-      </c>
-      <c r="K45" s="37">
-        <f t="shared" si="118"/>
-        <v>2</v>
-      </c>
-      <c r="L45" s="37">
-        <f t="shared" si="118"/>
-        <v>7</v>
-      </c>
-      <c r="M45" s="37">
-        <f t="shared" si="118"/>
-        <v>53.45</v>
-      </c>
-      <c r="N45" s="37">
-        <f t="shared" si="118"/>
-        <v>17.5</v>
-      </c>
-      <c r="O45" s="38">
-        <f t="shared" si="100"/>
-        <v>0.32740879326473338</v>
-      </c>
-      <c r="P45" s="37">
-        <f t="shared" ref="P45:Q45" si="119">SUM(P24:P27)</f>
-        <v>17.850000000000001</v>
-      </c>
-      <c r="Q45" s="37">
-        <f t="shared" si="119"/>
-        <v>3.5</v>
-      </c>
-      <c r="R45" s="38">
+        <v>6</v>
+      </c>
+      <c r="U45" s="38">
         <f t="shared" si="102"/>
-        <v>0.19607843137254902</v>
-      </c>
-      <c r="S45" s="37">
-        <f t="shared" ref="S45:T45" si="120">SUM(S24:S27)</f>
-        <v>15.399999999999999</v>
-      </c>
-      <c r="T45" s="37">
-        <f t="shared" si="120"/>
-        <v>6</v>
-      </c>
-      <c r="U45" s="38">
-        <f t="shared" si="104"/>
         <v>0.38961038961038963</v>
       </c>
       <c r="V45" s="39">
-        <f t="shared" si="105"/>
+        <f t="shared" si="103"/>
         <v>46.8</v>
       </c>
       <c r="Y45" s="26" t="s">
@@ -5454,75 +5456,75 @@
         <v>65</v>
       </c>
       <c r="E46" s="37">
-        <f t="shared" ref="E46:N46" si="121">SUM(E28:E31)</f>
+        <f t="shared" ref="E46:N46" si="119">SUM(E28:E31)</f>
         <v>56</v>
       </c>
       <c r="F46" s="37">
+        <f t="shared" si="119"/>
+        <v>42.2</v>
+      </c>
+      <c r="G46" s="37">
+        <f t="shared" si="119"/>
+        <v>16.2</v>
+      </c>
+      <c r="H46" s="37">
+        <f t="shared" si="119"/>
+        <v>26</v>
+      </c>
+      <c r="I46" s="37">
+        <f t="shared" si="119"/>
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="J46" s="37">
+        <f t="shared" si="119"/>
+        <v>5.7999999999999989</v>
+      </c>
+      <c r="K46" s="37">
+        <f t="shared" si="119"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="L46" s="37">
+        <f t="shared" si="119"/>
+        <v>6.7999999999999989</v>
+      </c>
+      <c r="M46" s="37">
+        <f t="shared" si="119"/>
+        <v>65.400000000000006</v>
+      </c>
+      <c r="N46" s="37">
+        <f t="shared" si="119"/>
+        <v>22</v>
+      </c>
+      <c r="O46" s="38">
+        <f t="shared" si="98"/>
+        <v>0.33639143730886845</v>
+      </c>
+      <c r="P46" s="37">
+        <f t="shared" ref="P46:Q46" si="120">SUM(P28:P31)</f>
+        <v>30.199999999999996</v>
+      </c>
+      <c r="Q46" s="37">
+        <f t="shared" si="120"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="R46" s="38">
+        <f t="shared" si="100"/>
+        <v>0.23841059602649006</v>
+      </c>
+      <c r="S46" s="37">
+        <f t="shared" ref="S46:T46" si="121">SUM(S28:S31)</f>
+        <v>10.4</v>
+      </c>
+      <c r="T46" s="37">
         <f t="shared" si="121"/>
-        <v>42.2</v>
-      </c>
-      <c r="G46" s="37">
-        <f t="shared" si="121"/>
-        <v>16.2</v>
-      </c>
-      <c r="H46" s="37">
-        <f t="shared" si="121"/>
-        <v>26</v>
-      </c>
-      <c r="I46" s="37">
-        <f t="shared" si="121"/>
-        <v>8.2000000000000011</v>
-      </c>
-      <c r="J46" s="37">
-        <f t="shared" si="121"/>
-        <v>5.7999999999999989</v>
-      </c>
-      <c r="K46" s="37">
-        <f t="shared" si="121"/>
-        <v>1.5999999999999999</v>
-      </c>
-      <c r="L46" s="37">
-        <f t="shared" si="121"/>
-        <v>6.7999999999999989</v>
-      </c>
-      <c r="M46" s="37">
-        <f t="shared" si="121"/>
-        <v>65.400000000000006</v>
-      </c>
-      <c r="N46" s="37">
-        <f t="shared" si="121"/>
-        <v>22</v>
-      </c>
-      <c r="O46" s="38">
-        <f t="shared" si="100"/>
-        <v>0.33639143730886845</v>
-      </c>
-      <c r="P46" s="37">
-        <f t="shared" ref="P46:Q46" si="122">SUM(P28:P31)</f>
-        <v>30.199999999999996</v>
-      </c>
-      <c r="Q46" s="37">
-        <f t="shared" si="122"/>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="R46" s="38">
+        <v>4</v>
+      </c>
+      <c r="U46" s="38">
         <f t="shared" si="102"/>
-        <v>0.23841059602649006</v>
-      </c>
-      <c r="S46" s="37">
-        <f t="shared" ref="S46:T46" si="123">SUM(S28:S31)</f>
-        <v>10.4</v>
-      </c>
-      <c r="T46" s="37">
-        <f t="shared" si="123"/>
-        <v>4</v>
-      </c>
-      <c r="U46" s="38">
-        <f t="shared" si="104"/>
         <v>0.38461538461538458</v>
       </c>
       <c r="V46" s="39">
-        <f t="shared" si="105"/>
+        <f t="shared" si="103"/>
         <v>44.8</v>
       </c>
       <c r="Y46" s="28" t="s">
@@ -5567,75 +5569,75 @@
         <v>67</v>
       </c>
       <c r="E47" s="37">
-        <f t="shared" ref="E47:N47" si="124">SUM(E32:E35)</f>
+        <f t="shared" ref="E47:N47" si="122">SUM(E32:E35)</f>
         <v>57.9</v>
       </c>
       <c r="F47" s="37">
+        <f t="shared" si="122"/>
+        <v>35.449999999999996</v>
+      </c>
+      <c r="G47" s="37">
+        <f t="shared" si="122"/>
+        <v>9.85</v>
+      </c>
+      <c r="H47" s="37">
+        <f t="shared" si="122"/>
+        <v>25.6</v>
+      </c>
+      <c r="I47" s="37">
+        <f t="shared" si="122"/>
+        <v>11.200000000000001</v>
+      </c>
+      <c r="J47" s="37">
+        <f t="shared" si="122"/>
+        <v>4.3999999999999995</v>
+      </c>
+      <c r="K47" s="37">
+        <f t="shared" si="122"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L47" s="37">
+        <f t="shared" si="122"/>
+        <v>7.4499999999999993</v>
+      </c>
+      <c r="M47" s="37">
+        <f t="shared" si="122"/>
+        <v>56.699999999999996</v>
+      </c>
+      <c r="N47" s="37">
+        <f t="shared" si="122"/>
+        <v>23.700000000000003</v>
+      </c>
+      <c r="O47" s="38">
+        <f t="shared" si="98"/>
+        <v>0.41798941798941808</v>
+      </c>
+      <c r="P47" s="37">
+        <f t="shared" ref="P47:Q47" si="123">SUM(P32:P35)</f>
+        <v>13.799999999999999</v>
+      </c>
+      <c r="Q47" s="37">
+        <f t="shared" si="123"/>
+        <v>2.65</v>
+      </c>
+      <c r="R47" s="38">
+        <f t="shared" si="100"/>
+        <v>0.1920289855072464</v>
+      </c>
+      <c r="S47" s="37">
+        <f t="shared" ref="S47:T47" si="124">SUM(S32:S35)</f>
+        <v>13.25</v>
+      </c>
+      <c r="T47" s="37">
         <f t="shared" si="124"/>
-        <v>35.449999999999996</v>
-      </c>
-      <c r="G47" s="37">
-        <f t="shared" si="124"/>
-        <v>9.85</v>
-      </c>
-      <c r="H47" s="37">
-        <f t="shared" si="124"/>
-        <v>25.6</v>
-      </c>
-      <c r="I47" s="37">
-        <f t="shared" si="124"/>
-        <v>11.200000000000001</v>
-      </c>
-      <c r="J47" s="37">
-        <f t="shared" si="124"/>
-        <v>4.3999999999999995</v>
-      </c>
-      <c r="K47" s="37">
-        <f t="shared" si="124"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="L47" s="37">
-        <f t="shared" si="124"/>
-        <v>7.4499999999999993</v>
-      </c>
-      <c r="M47" s="37">
-        <f t="shared" si="124"/>
-        <v>56.699999999999996</v>
-      </c>
-      <c r="N47" s="37">
-        <f t="shared" si="124"/>
-        <v>23.700000000000003</v>
-      </c>
-      <c r="O47" s="38">
-        <f t="shared" si="100"/>
-        <v>0.41798941798941808</v>
-      </c>
-      <c r="P47" s="37">
-        <f t="shared" ref="P47:Q47" si="125">SUM(P32:P35)</f>
-        <v>13.799999999999999</v>
-      </c>
-      <c r="Q47" s="37">
-        <f t="shared" si="125"/>
-        <v>2.65</v>
-      </c>
-      <c r="R47" s="38">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="U47" s="38">
         <f t="shared" si="102"/>
-        <v>0.1920289855072464</v>
-      </c>
-      <c r="S47" s="37">
-        <f t="shared" ref="S47:T47" si="126">SUM(S32:S35)</f>
-        <v>13.25</v>
-      </c>
-      <c r="T47" s="37">
-        <f t="shared" si="126"/>
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="U47" s="38">
-        <f t="shared" si="104"/>
         <v>0.60754716981132084</v>
       </c>
       <c r="V47" s="39">
-        <f t="shared" si="105"/>
+        <f t="shared" si="103"/>
         <v>49.2</v>
       </c>
       <c r="Y47" s="30" t="s">
@@ -5679,75 +5681,75 @@
         <v>68</v>
       </c>
       <c r="E48" s="42">
-        <f t="shared" ref="E48:V48" si="127">AVERAGE(E40:E47)</f>
+        <f t="shared" ref="E48:V48" si="125">AVERAGE(E40:E47)</f>
         <v>49.949999999999996</v>
       </c>
       <c r="F48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>35.912500000000001</v>
       </c>
       <c r="G48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>10.018749999999999</v>
       </c>
       <c r="H48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>25.893749999999997</v>
       </c>
       <c r="I48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>8.6999999999999993</v>
       </c>
       <c r="J48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>4.4187499999999993</v>
       </c>
       <c r="K48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>2.4937500000000004</v>
       </c>
       <c r="L48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>7.2249999999999996</v>
       </c>
       <c r="M48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>58.631250000000001</v>
       </c>
       <c r="N48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>19.850000000000001</v>
       </c>
       <c r="O48" s="35">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>0.3388759349416201</v>
       </c>
       <c r="P48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>21.7</v>
       </c>
       <c r="Q48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>4.6874999999999991</v>
       </c>
       <c r="R48" s="35">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>0.2147429871821899</v>
       </c>
       <c r="S48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>11.193750000000001</v>
       </c>
       <c r="T48" s="42">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>5.6062499999999993</v>
       </c>
       <c r="U48" s="35">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>0.50727593481006605</v>
       </c>
       <c r="V48" s="43">
-        <f t="shared" si="127"/>
+        <f t="shared" si="125"/>
         <v>49.875</v>
       </c>
     </row>
@@ -21405,7 +21407,7 @@
   <dimension ref="A1:AH977"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>